<commit_message>
rectify README of SHADE & LSHADE
</commit_message>
<xml_diff>
--- a/DE_extension_ExperimentResults.xlsx
+++ b/DE_extension_ExperimentResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MyCode\VisualStudio\meta_algo\DE_extension_to_CEC2014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8413C1DB-A83B-4975-AE66-ED3C0F4DAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6C8719-E385-48B8-9352-F7C0E45309F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50E21A78-8C48-40D2-9105-B406553DA780}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{50E21A78-8C48-40D2-9105-B406553DA780}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>f1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -293,6 +293,10 @@
   </si>
   <si>
     <t>L-SHADE w/o archive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXPERIMENTAL RESULTS OF 50-DIMENSIONAL PROBLEMS CEC2014 f1– f30, AVERAGED OVER 51 INDEPENDENT RUNS, EVALUATION D*10000 TIMES</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -303,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,15 +442,6 @@
     <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -460,6 +455,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,13 +800,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A90AD3-D743-4E65-B2C8-F3B5C98AC2E6}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.08984375" style="1" bestFit="1" customWidth="1"/>
@@ -819,20 +823,20 @@
     <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.4">
+      <c r="B1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -859,13 +863,13 @@
       <c r="J2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="11"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -874,7 +878,7 @@
       <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="6">
         <v>138318000</v>
       </c>
       <c r="E3" s="4">
@@ -895,20 +899,20 @@
       <c r="J3" s="5">
         <v>2.8659399999999997E-17</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>1261860</v>
       </c>
       <c r="E4" s="4">
@@ -929,20 +933,20 @@
       <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="L4" s="13"/>
+      <c r="L4" s="10"/>
       <c r="M4" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>1255.78</v>
       </c>
       <c r="E5" s="4">
@@ -964,8 +968,8 @@
         <v>7.8764400000000004E-29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -974,7 +978,7 @@
       <c r="C6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>136.71700000000001</v>
       </c>
       <c r="E6" s="4">
@@ -996,8 +1000,8 @@
         <v>4.6460900000000003E-11</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1026,8 +1030,8 @@
         <v>20.157499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="12"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1046,25 +1050,25 @@
       <c r="G8" s="4">
         <v>5.6036099999999998</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>3.97716</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>8.7979099999999999</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="7">
         <v>7.1407699999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <v>0.27936899999999998</v>
       </c>
       <c r="E9" s="4">
@@ -1086,15 +1090,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <v>126.812</v>
       </c>
       <c r="E10" s="4">
@@ -1116,15 +1120,15 @@
         <v>6.9661100000000001E-16</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <v>195.85400000000001</v>
       </c>
       <c r="E11" s="4">
@@ -1142,19 +1146,19 @@
       <c r="I11" s="4">
         <v>18.2437</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="7">
         <v>18.7578</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="12"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <v>4559.67</v>
       </c>
       <c r="E12" s="4">
@@ -1176,8 +1180,8 @@
         <v>3.41147</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="12"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1202,12 +1206,12 @@
       <c r="I13" s="4">
         <v>1394.56</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="7">
         <v>1329.44</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="7"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1232,12 +1236,12 @@
       <c r="I14" s="4">
         <v>0.18904399999999999</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="7">
         <v>0.18802099999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="12"/>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1262,12 +1266,12 @@
       <c r="I15" s="4">
         <v>0.15492300000000001</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="7">
         <v>0.17369399999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="7"/>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1296,15 +1300,15 @@
         <v>0.22914300000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="12"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="6">
         <v>18.3794</v>
       </c>
       <c r="E17" s="4">
@@ -1322,12 +1326,12 @@
       <c r="I17" s="4">
         <v>2.4412099999999999</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="7">
         <v>2.5117400000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1356,8 +1360,8 @@
         <v>9.0694300000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1366,13 +1370,13 @@
       <c r="C19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="6">
         <v>3701300</v>
       </c>
       <c r="E19" s="4">
         <v>267.05500000000001</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>296.529</v>
       </c>
       <c r="G19" s="4">
@@ -1388,15 +1392,15 @@
         <v>420.99900000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="6">
         <v>165480</v>
       </c>
       <c r="E20" s="4">
@@ -1414,12 +1418,12 @@
       <c r="I20" s="4">
         <v>9.1368200000000002</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="7">
         <v>16.4497</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" s="12"/>
       <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
@@ -1444,12 +1448,12 @@
       <c r="I21" s="4">
         <v>3.60175</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="7">
         <v>4.0993399999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="7"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22" s="12"/>
       <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1478,15 +1482,15 @@
         <v>3.8368699999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="7"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23" s="12"/>
       <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="6">
         <v>521494</v>
       </c>
       <c r="E23" s="4">
@@ -1504,12 +1508,12 @@
       <c r="I23" s="4">
         <v>112.26600000000001</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="7">
         <v>160.947</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="7"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
@@ -1534,12 +1538,12 @@
       <c r="I24" s="4">
         <v>48.537399999999998</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="7">
         <v>55.078099999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1570,8 +1574,8 @@
         <v>315.24400000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="7"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
@@ -1600,8 +1604,8 @@
         <v>223.58099999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27" s="12"/>
       <c r="B27" s="3" t="s">
         <v>30</v>
       </c>
@@ -1630,8 +1634,8 @@
         <v>202.63399999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" s="12"/>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
@@ -1660,8 +1664,8 @@
         <v>100.15900000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29" s="12"/>
       <c r="B29" s="3" t="s">
         <v>32</v>
       </c>
@@ -1690,8 +1694,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30" s="12"/>
       <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
@@ -1720,15 +1724,15 @@
         <v>800.97199999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="12"/>
       <c r="B31" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="6">
         <v>21109.5</v>
       </c>
       <c r="E31" s="4">
@@ -1750,15 +1754,15 @@
         <v>717.27800000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" s="12"/>
       <c r="B32" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="6">
         <v>11050.8</v>
       </c>
       <c r="E32" s="4">
@@ -1773,15 +1777,969 @@
       <c r="H32" s="4">
         <v>1272.58</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="7">
         <v>706.89800000000002</v>
       </c>
       <c r="J32" s="4">
         <v>1619.65</v>
       </c>
     </row>
+    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="B34" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="6">
+        <v>138318000</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4.3666799999999999E-10</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1.4385299999999999E-11</v>
+      </c>
+      <c r="G36" s="4">
+        <v>9377.2199999999993</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2553.9899999999998</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2.3601800000000002E-6</v>
+      </c>
+      <c r="J36" s="5">
+        <v>2.8659399999999997E-17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A37" s="12"/>
+      <c r="B37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1261860</v>
+      </c>
+      <c r="E37" s="4">
+        <v>1.10719E-16</v>
+      </c>
+      <c r="F37" s="4">
+        <v>7.6855300000000001E-14</v>
+      </c>
+      <c r="G37" s="4">
+        <v>9.3305599999999997E-9</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1.36279E-7</v>
+      </c>
+      <c r="I37" s="4">
+        <v>1.2844E-21</v>
+      </c>
+      <c r="J37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A38" s="12"/>
+      <c r="B38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1255.78</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.13309399999999999</v>
+      </c>
+      <c r="F38" s="4">
+        <v>4.0321300000000004</v>
+      </c>
+      <c r="G38" s="4">
+        <v>2.6414499999999999E-11</v>
+      </c>
+      <c r="H38" s="4">
+        <v>7.1997499999999999E-10</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1.1454200000000001E-27</v>
+      </c>
+      <c r="J38" s="5">
+        <v>7.8764400000000004E-29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A39" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="6">
+        <v>136.71700000000001</v>
+      </c>
+      <c r="E39" s="4">
+        <v>12.5573</v>
+      </c>
+      <c r="F39" s="4">
+        <v>3.1390500000000001</v>
+      </c>
+      <c r="G39" s="4">
+        <v>71.248800000000003</v>
+      </c>
+      <c r="H39" s="4">
+        <v>51.398600000000002</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0.25564500000000001</v>
+      </c>
+      <c r="J39" s="5">
+        <v>4.6460900000000003E-11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A40" s="12"/>
+      <c r="B40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="4">
+        <v>20.910599999999999</v>
+      </c>
+      <c r="E40" s="4">
+        <v>20.467700000000001</v>
+      </c>
+      <c r="F40" s="4">
+        <v>20.457599999999999</v>
+      </c>
+      <c r="G40" s="4">
+        <v>20.509799999999998</v>
+      </c>
+      <c r="H40" s="4">
+        <v>20.496200000000002</v>
+      </c>
+      <c r="I40" s="4">
+        <v>20.160499999999999</v>
+      </c>
+      <c r="J40" s="4">
+        <v>20.157499999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A41" s="12"/>
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="4">
+        <v>32.485999999999997</v>
+      </c>
+      <c r="E41" s="4">
+        <v>13.7882</v>
+      </c>
+      <c r="F41" s="4">
+        <v>14.163399999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>5.6036099999999998</v>
+      </c>
+      <c r="H41" s="7">
+        <v>3.97716</v>
+      </c>
+      <c r="I41" s="7">
+        <v>8.7979099999999999</v>
+      </c>
+      <c r="J41" s="7">
+        <v>7.1407699999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A42" s="12"/>
+      <c r="B42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0.27936899999999998</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1.74153E-17</v>
+      </c>
+      <c r="F42" s="4">
+        <v>4.0991200000000002E-15</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1.95922E-17</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A43" s="12"/>
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="6">
+        <v>126.812</v>
+      </c>
+      <c r="E43" s="4">
+        <v>12.1471</v>
+      </c>
+      <c r="F43" s="4">
+        <v>12.186500000000001</v>
+      </c>
+      <c r="G43" s="4">
+        <v>28.178799999999999</v>
+      </c>
+      <c r="H43" s="4">
+        <v>28.884799999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>5.4335599999999999E-15</v>
+      </c>
+      <c r="J43" s="5">
+        <v>6.9661100000000001E-16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A44" s="12"/>
+      <c r="B44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="6">
+        <v>195.85400000000001</v>
+      </c>
+      <c r="E44" s="4">
+        <v>61.351399999999998</v>
+      </c>
+      <c r="F44" s="4">
+        <v>64.094099999999997</v>
+      </c>
+      <c r="G44" s="4">
+        <v>77.900899999999993</v>
+      </c>
+      <c r="H44" s="4">
+        <v>78.036600000000007</v>
+      </c>
+      <c r="I44" s="4">
+        <v>18.2437</v>
+      </c>
+      <c r="J44" s="7">
+        <v>18.7578</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A45" s="12"/>
+      <c r="B45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="6">
+        <v>4559.67</v>
+      </c>
+      <c r="E45" s="4">
+        <v>407.09100000000001</v>
+      </c>
+      <c r="F45" s="4">
+        <v>406.67399999999998</v>
+      </c>
+      <c r="G45" s="4">
+        <v>965.64</v>
+      </c>
+      <c r="H45" s="4">
+        <v>990.35900000000004</v>
+      </c>
+      <c r="I45" s="4">
+        <v>4.7009699999999999</v>
+      </c>
+      <c r="J45" s="5">
+        <v>3.41147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A46" s="12"/>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="4">
+        <v>6639.53</v>
+      </c>
+      <c r="E46" s="4">
+        <v>3501.42</v>
+      </c>
+      <c r="F46" s="4">
+        <v>3510.21</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3898.56</v>
+      </c>
+      <c r="H46" s="4">
+        <v>3837.16</v>
+      </c>
+      <c r="I46" s="4">
+        <v>1394.56</v>
+      </c>
+      <c r="J46" s="7">
+        <v>1329.44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A47" s="12"/>
+      <c r="B47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="4">
+        <v>2.1954400000000001</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0.69625899999999996</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.69176899999999997</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.76464500000000002</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.769038</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0.18904399999999999</v>
+      </c>
+      <c r="J47" s="7">
+        <v>0.18802099999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A48" s="12"/>
+      <c r="B48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.44996700000000001</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0.21293899999999999</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.22465199999999999</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0.21718799999999999</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.228406</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0.15492300000000001</v>
+      </c>
+      <c r="J48" s="7">
+        <v>0.17369399999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A49" s="12"/>
+      <c r="B49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.278949</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.236981</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0.23897699999999999</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.227384</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.247251</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0.21333299999999999</v>
+      </c>
+      <c r="J49" s="4">
+        <v>0.22914300000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A50" s="12"/>
+      <c r="B50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="6">
+        <v>18.3794</v>
+      </c>
+      <c r="E50" s="4">
+        <v>6.9556100000000001</v>
+      </c>
+      <c r="F50" s="4">
+        <v>7.0234199999999998</v>
+      </c>
+      <c r="G50" s="4">
+        <v>8.9435000000000002</v>
+      </c>
+      <c r="H50" s="4">
+        <v>9.0207599999999992</v>
+      </c>
+      <c r="I50" s="4">
+        <v>2.4412099999999999</v>
+      </c>
+      <c r="J50" s="7">
+        <v>2.5117400000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A51" s="12"/>
+      <c r="B51" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="4">
+        <v>12.6866</v>
+      </c>
+      <c r="E51" s="4">
+        <v>10.717000000000001</v>
+      </c>
+      <c r="F51" s="4">
+        <v>10.689399999999999</v>
+      </c>
+      <c r="G51" s="4">
+        <v>11.003500000000001</v>
+      </c>
+      <c r="H51" s="4">
+        <v>10.989000000000001</v>
+      </c>
+      <c r="I51" s="4">
+        <v>9.1163100000000004</v>
+      </c>
+      <c r="J51" s="4">
+        <v>9.0694300000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A52" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="6">
+        <v>3701300</v>
+      </c>
+      <c r="E52" s="4">
+        <v>267.05500000000001</v>
+      </c>
+      <c r="F52" s="7">
+        <v>296.529</v>
+      </c>
+      <c r="G52" s="4">
+        <v>406.94299999999998</v>
+      </c>
+      <c r="H52" s="4">
+        <v>383.846</v>
+      </c>
+      <c r="I52" s="4">
+        <v>247.35499999999999</v>
+      </c>
+      <c r="J52" s="4">
+        <v>420.99900000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A53" s="12"/>
+      <c r="B53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="6">
+        <v>165480</v>
+      </c>
+      <c r="E53" s="4">
+        <v>21.988099999999999</v>
+      </c>
+      <c r="F53" s="4">
+        <v>20.677</v>
+      </c>
+      <c r="G53" s="4">
+        <v>38.487099999999998</v>
+      </c>
+      <c r="H53" s="4">
+        <v>40.285899999999998</v>
+      </c>
+      <c r="I53" s="4">
+        <v>9.1368200000000002</v>
+      </c>
+      <c r="J53" s="7">
+        <v>16.4497</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A54" s="12"/>
+      <c r="B54" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="4">
+        <v>11.8787</v>
+      </c>
+      <c r="E54" s="4">
+        <v>5.0997899999999996</v>
+      </c>
+      <c r="F54" s="4">
+        <v>4.8965300000000003</v>
+      </c>
+      <c r="G54" s="4">
+        <v>5.2138999999999998</v>
+      </c>
+      <c r="H54" s="4">
+        <v>5.2250199999999998</v>
+      </c>
+      <c r="I54" s="4">
+        <v>3.60175</v>
+      </c>
+      <c r="J54" s="7">
+        <v>4.0993399999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A55" s="12"/>
+      <c r="B55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="4">
+        <v>4343.1000000000004</v>
+      </c>
+      <c r="E55" s="4">
+        <v>291.53199999999998</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1644.22</v>
+      </c>
+      <c r="G55" s="4">
+        <v>24.012</v>
+      </c>
+      <c r="H55" s="4">
+        <v>23.332599999999999</v>
+      </c>
+      <c r="I55" s="4">
+        <v>4.8087799999999996</v>
+      </c>
+      <c r="J55" s="5">
+        <v>3.8368699999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A56" s="12"/>
+      <c r="B56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="6">
+        <v>521494</v>
+      </c>
+      <c r="E56" s="4">
+        <v>337.59199999999998</v>
+      </c>
+      <c r="F56" s="4">
+        <v>341.53899999999999</v>
+      </c>
+      <c r="G56" s="4">
+        <v>464.964</v>
+      </c>
+      <c r="H56" s="4">
+        <v>504.87299999999999</v>
+      </c>
+      <c r="I56" s="4">
+        <v>112.26600000000001</v>
+      </c>
+      <c r="J56" s="7">
+        <v>160.947</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A57" s="12"/>
+      <c r="B57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="4">
+        <v>322.58100000000002</v>
+      </c>
+      <c r="E57" s="4">
+        <v>205.779</v>
+      </c>
+      <c r="F57" s="4">
+        <v>194.852</v>
+      </c>
+      <c r="G57" s="4">
+        <v>182.31800000000001</v>
+      </c>
+      <c r="H57" s="4">
+        <v>178.47900000000001</v>
+      </c>
+      <c r="I57" s="4">
+        <v>48.537399999999998</v>
+      </c>
+      <c r="J57" s="7">
+        <v>55.078099999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A58" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="4">
+        <v>315.392</v>
+      </c>
+      <c r="E58" s="4">
+        <v>315.24400000000003</v>
+      </c>
+      <c r="F58" s="4">
+        <v>315.24400000000003</v>
+      </c>
+      <c r="G58" s="4">
+        <v>315.24400000000003</v>
+      </c>
+      <c r="H58" s="4">
+        <v>315.24400000000003</v>
+      </c>
+      <c r="I58" s="4">
+        <v>315.24400000000003</v>
+      </c>
+      <c r="J58" s="4">
+        <v>315.24400000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A59" s="12"/>
+      <c r="B59" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="4">
+        <v>227.26</v>
+      </c>
+      <c r="E59" s="4">
+        <v>223.59299999999999</v>
+      </c>
+      <c r="F59" s="4">
+        <v>223.49</v>
+      </c>
+      <c r="G59" s="4">
+        <v>223.59899999999999</v>
+      </c>
+      <c r="H59" s="4">
+        <v>223.59</v>
+      </c>
+      <c r="I59" s="4">
+        <v>223.93899999999999</v>
+      </c>
+      <c r="J59" s="4">
+        <v>223.58099999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A60" s="12"/>
+      <c r="B60" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" s="4">
+        <v>230.131</v>
+      </c>
+      <c r="E60" s="4">
+        <v>202.98599999999999</v>
+      </c>
+      <c r="F60" s="4">
+        <v>202.78</v>
+      </c>
+      <c r="G60" s="4">
+        <v>203.923</v>
+      </c>
+      <c r="H60" s="4">
+        <v>203.285</v>
+      </c>
+      <c r="I60" s="4">
+        <v>202.66</v>
+      </c>
+      <c r="J60" s="4">
+        <v>202.63399999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A61" s="12"/>
+      <c r="B61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="4">
+        <v>100.449</v>
+      </c>
+      <c r="E61" s="4">
+        <v>100.23699999999999</v>
+      </c>
+      <c r="F61" s="4">
+        <v>100.241</v>
+      </c>
+      <c r="G61" s="4">
+        <v>100.23099999999999</v>
+      </c>
+      <c r="H61" s="4">
+        <v>100.233</v>
+      </c>
+      <c r="I61" s="4">
+        <v>100.154</v>
+      </c>
+      <c r="J61" s="4">
+        <v>100.15900000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A62" s="12"/>
+      <c r="B62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="4">
+        <v>592.82799999999997</v>
+      </c>
+      <c r="E62" s="4">
+        <v>313.06299999999999</v>
+      </c>
+      <c r="F62" s="4">
+        <v>311.358</v>
+      </c>
+      <c r="G62" s="4">
+        <v>330.34100000000001</v>
+      </c>
+      <c r="H62" s="4">
+        <v>304.38799999999998</v>
+      </c>
+      <c r="I62" s="4">
+        <v>319.98099999999999</v>
+      </c>
+      <c r="J62" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A63" s="12"/>
+      <c r="B63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="4">
+        <v>1005.76</v>
+      </c>
+      <c r="E63" s="4">
+        <v>826.81100000000004</v>
+      </c>
+      <c r="F63" s="4">
+        <v>821.92399999999998</v>
+      </c>
+      <c r="G63" s="4">
+        <v>833.69600000000003</v>
+      </c>
+      <c r="H63" s="4">
+        <v>806.755</v>
+      </c>
+      <c r="I63" s="4">
+        <v>802.56799999999998</v>
+      </c>
+      <c r="J63" s="4">
+        <v>800.97199999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A64" s="12"/>
+      <c r="B64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="6">
+        <v>21109.5</v>
+      </c>
+      <c r="E64" s="4">
+        <v>716.07299999999998</v>
+      </c>
+      <c r="F64" s="4">
+        <v>717.495</v>
+      </c>
+      <c r="G64" s="4">
+        <v>716.72900000000004</v>
+      </c>
+      <c r="H64" s="4">
+        <v>717.16600000000005</v>
+      </c>
+      <c r="I64" s="4">
+        <v>708.88</v>
+      </c>
+      <c r="J64" s="4">
+        <v>717.27800000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A65" s="12"/>
+      <c r="B65" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" s="6">
+        <v>11050.8</v>
+      </c>
+      <c r="E65" s="4">
+        <v>863.64</v>
+      </c>
+      <c r="F65" s="4">
+        <v>1060.58</v>
+      </c>
+      <c r="G65" s="4">
+        <v>1156.8900000000001</v>
+      </c>
+      <c r="H65" s="4">
+        <v>1272.58</v>
+      </c>
+      <c r="I65" s="7">
+        <v>706.89800000000002</v>
+      </c>
+      <c r="J65" s="4">
+        <v>1619.65</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A51"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A58:A65"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A18"/>
     <mergeCell ref="A19:A24"/>

</xml_diff>

<commit_message>
add results in excel
</commit_message>
<xml_diff>
--- a/DE_extension_ExperimentResults.xlsx
+++ b/DE_extension_ExperimentResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MyCode\VisualStudio\meta_algo\DE_extension_to_CEC2014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6C8719-E385-48B8-9352-F7C0E45309F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF55D11-6C58-4DAE-8670-0AA02816BA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{50E21A78-8C48-40D2-9105-B406553DA780}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50E21A78-8C48-40D2-9105-B406553DA780}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="79">
   <si>
     <t>f1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,6 +297,14 @@
   </si>
   <si>
     <t>EXPERIMENTAL RESULTS OF 50-DIMENSIONAL PROBLEMS CEC2014 f1– f30, AVERAGED OVER 51 INDEPENDENT RUNS, EVALUATION D*10000 TIMES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXPERIMENTAL RESULTS OF 100-DIMENSIONAL PROBLEMS CEC2014 f1– f30, AVERAGED OVER 51 INDEPENDENT RUNS, EVALUATION D*10000 TIMES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXPERIMENTAL RESULTS OF 10-DIMENSIONAL PROBLEMS CEC2014 f1– f30, AVERAGED OVER 51 INDEPENDENT RUNS, EVALUATION D*10000 TIMES</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -307,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,7 +431,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -463,7 +471,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -800,13 +817,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A90AD3-D743-4E65-B2C8-F3B5C98AC2E6}">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:J34"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.08984375" style="1" bestFit="1" customWidth="1"/>
@@ -823,7 +840,8 @@
     <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="18">
+      <c r="A1" s="3"/>
       <c r="B1" s="13" t="s">
         <v>73</v>
       </c>
@@ -836,7 +854,7 @@
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -868,7 +886,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
         <v>36</v>
       </c>
@@ -904,7 +922,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13">
       <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -938,7 +956,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13">
       <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -968,7 +986,7 @@
         <v>7.8764400000000004E-29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="17" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>37</v>
       </c>
@@ -1000,7 +1018,7 @@
         <v>4.6460900000000003E-11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13">
       <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1030,7 +1048,7 @@
         <v>20.157499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13">
       <c r="A8" s="12"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -1060,7 +1078,7 @@
         <v>7.1407699999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13">
       <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -1090,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13">
       <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -1120,7 +1138,7 @@
         <v>6.9661100000000001E-16</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13">
       <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -1150,7 +1168,7 @@
         <v>18.7578</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13">
       <c r="A12" s="12"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -1180,7 +1198,7 @@
         <v>3.41147</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13">
       <c r="A13" s="12"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -1210,7 +1228,7 @@
         <v>1329.44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13">
       <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -1240,7 +1258,7 @@
         <v>0.18802099999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13">
       <c r="A15" s="12"/>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -1270,7 +1288,7 @@
         <v>0.17369399999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13">
       <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
@@ -1300,7 +1318,7 @@
         <v>0.22914300000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10">
       <c r="A17" s="12"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
@@ -1330,7 +1348,7 @@
         <v>2.5117400000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10">
       <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -1360,7 +1378,7 @@
         <v>9.0694300000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10">
       <c r="A19" s="11" t="s">
         <v>38</v>
       </c>
@@ -1392,7 +1410,7 @@
         <v>420.99900000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10">
       <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>23</v>
@@ -1422,7 +1440,7 @@
         <v>16.4497</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10">
       <c r="A21" s="12"/>
       <c r="B21" s="3" t="s">
         <v>24</v>
@@ -1452,7 +1470,7 @@
         <v>4.0993399999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10">
       <c r="A22" s="12"/>
       <c r="B22" s="3" t="s">
         <v>25</v>
@@ -1482,7 +1500,7 @@
         <v>3.8368699999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10">
       <c r="A23" s="12"/>
       <c r="B23" s="3" t="s">
         <v>26</v>
@@ -1512,7 +1530,7 @@
         <v>160.947</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10">
       <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
         <v>27</v>
@@ -1542,7 +1560,7 @@
         <v>55.078099999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10">
       <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
@@ -1574,7 +1592,7 @@
         <v>315.24400000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10">
       <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
         <v>29</v>
@@ -1604,7 +1622,7 @@
         <v>223.58099999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10">
       <c r="A27" s="12"/>
       <c r="B27" s="3" t="s">
         <v>30</v>
@@ -1634,7 +1652,7 @@
         <v>202.63399999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10">
       <c r="A28" s="12"/>
       <c r="B28" s="3" t="s">
         <v>31</v>
@@ -1664,7 +1682,7 @@
         <v>100.15900000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10">
       <c r="A29" s="12"/>
       <c r="B29" s="3" t="s">
         <v>32</v>
@@ -1694,7 +1712,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10">
       <c r="A30" s="12"/>
       <c r="B30" s="3" t="s">
         <v>33</v>
@@ -1724,7 +1742,7 @@
         <v>800.97199999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10">
       <c r="A31" s="12"/>
       <c r="B31" s="3" t="s">
         <v>34</v>
@@ -1754,7 +1772,7 @@
         <v>717.27800000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10">
       <c r="A32" s="12"/>
       <c r="B32" s="3" t="s">
         <v>35</v>
@@ -1784,7 +1802,8 @@
         <v>1619.65</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" ht="18">
+      <c r="A34" s="3"/>
       <c r="B34" s="13" t="s">
         <v>76</v>
       </c>
@@ -1797,7 +1816,7 @@
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
@@ -1825,7 +1844,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10">
       <c r="A36" s="11" t="s">
         <v>36</v>
       </c>
@@ -1835,29 +1854,29 @@
       <c r="C36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="6">
-        <v>138318000</v>
-      </c>
-      <c r="E36" s="4">
-        <v>4.3666799999999999E-10</v>
-      </c>
-      <c r="F36" s="4">
-        <v>1.4385299999999999E-11</v>
-      </c>
-      <c r="G36" s="4">
-        <v>9377.2199999999993</v>
-      </c>
-      <c r="H36" s="4">
-        <v>2553.9899999999998</v>
-      </c>
-      <c r="I36" s="4">
-        <v>2.3601800000000002E-6</v>
-      </c>
-      <c r="J36" s="5">
-        <v>2.8659399999999997E-17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D36" s="14">
+        <v>485320000</v>
+      </c>
+      <c r="E36" s="14">
+        <v>6540910</v>
+      </c>
+      <c r="F36" s="14">
+        <v>6949670</v>
+      </c>
+      <c r="G36" s="14">
+        <v>1264920</v>
+      </c>
+      <c r="H36" s="14">
+        <v>729528</v>
+      </c>
+      <c r="I36" s="14">
+        <v>1264920</v>
+      </c>
+      <c r="J36" s="14">
+        <v>729528</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="12"/>
       <c r="B37" s="3" t="s">
         <v>1</v>
@@ -1865,29 +1884,29 @@
       <c r="C37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="6">
-        <v>1261860</v>
-      </c>
-      <c r="E37" s="4">
-        <v>1.10719E-16</v>
-      </c>
-      <c r="F37" s="4">
-        <v>7.6855300000000001E-14</v>
-      </c>
-      <c r="G37" s="4">
-        <v>9.3305599999999997E-9</v>
-      </c>
-      <c r="H37" s="4">
-        <v>1.36279E-7</v>
-      </c>
-      <c r="I37" s="4">
-        <v>1.2844E-21</v>
-      </c>
-      <c r="J37" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D37" s="14">
+        <v>376403000</v>
+      </c>
+      <c r="E37" s="14">
+        <v>3401.12</v>
+      </c>
+      <c r="F37" s="14">
+        <v>3638.82</v>
+      </c>
+      <c r="G37" s="14">
+        <v>3268.32</v>
+      </c>
+      <c r="H37" s="14">
+        <v>94.282399999999996</v>
+      </c>
+      <c r="I37" s="14">
+        <v>3268.32</v>
+      </c>
+      <c r="J37" s="14">
+        <v>94.282399999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="12"/>
       <c r="B38" s="3" t="s">
         <v>2</v>
@@ -1895,29 +1914,29 @@
       <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="6">
-        <v>1255.78</v>
-      </c>
-      <c r="E38" s="4">
-        <v>0.13309399999999999</v>
-      </c>
-      <c r="F38" s="4">
-        <v>4.0321300000000004</v>
-      </c>
-      <c r="G38" s="4">
-        <v>2.6414499999999999E-11</v>
-      </c>
-      <c r="H38" s="4">
-        <v>7.1997499999999999E-10</v>
-      </c>
-      <c r="I38" s="4">
-        <v>1.1454200000000001E-27</v>
-      </c>
-      <c r="J38" s="5">
-        <v>7.8764400000000004E-29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D38" s="14">
+        <v>161642</v>
+      </c>
+      <c r="E38" s="14">
+        <v>26493.7</v>
+      </c>
+      <c r="F38" s="14">
+        <v>25788.6</v>
+      </c>
+      <c r="G38" s="14">
+        <v>2.20017E-7</v>
+      </c>
+      <c r="H38" s="14">
+        <v>4.30221E-10</v>
+      </c>
+      <c r="I38" s="14">
+        <v>2.20017E-7</v>
+      </c>
+      <c r="J38" s="14">
+        <v>4.30221E-10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="11" t="s">
         <v>37</v>
       </c>
@@ -1927,29 +1946,29 @@
       <c r="C39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="6">
-        <v>136.71700000000001</v>
-      </c>
-      <c r="E39" s="4">
-        <v>12.5573</v>
-      </c>
-      <c r="F39" s="4">
-        <v>3.1390500000000001</v>
-      </c>
-      <c r="G39" s="4">
-        <v>71.248800000000003</v>
-      </c>
-      <c r="H39" s="4">
-        <v>51.398600000000002</v>
-      </c>
-      <c r="I39" s="4">
-        <v>0.25564500000000001</v>
-      </c>
-      <c r="J39" s="5">
-        <v>4.6460900000000003E-11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D39" s="14">
+        <v>243.351</v>
+      </c>
+      <c r="E39" s="14">
+        <v>96.700299999999999</v>
+      </c>
+      <c r="F39" s="14">
+        <v>95.371300000000005</v>
+      </c>
+      <c r="G39" s="14">
+        <v>96.091300000000004</v>
+      </c>
+      <c r="H39" s="14">
+        <v>94.047300000000007</v>
+      </c>
+      <c r="I39" s="14">
+        <v>96.091300000000004</v>
+      </c>
+      <c r="J39" s="14">
+        <v>94.047300000000007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="12"/>
       <c r="B40" s="3" t="s">
         <v>4</v>
@@ -1957,29 +1976,29 @@
       <c r="C40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="4">
-        <v>20.910599999999999</v>
-      </c>
-      <c r="E40" s="4">
-        <v>20.467700000000001</v>
-      </c>
-      <c r="F40" s="4">
-        <v>20.457599999999999</v>
-      </c>
-      <c r="G40" s="4">
-        <v>20.509799999999998</v>
-      </c>
-      <c r="H40" s="4">
-        <v>20.496200000000002</v>
-      </c>
-      <c r="I40" s="4">
-        <v>20.160499999999999</v>
-      </c>
-      <c r="J40" s="4">
-        <v>20.157499999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D40" s="14">
+        <v>21.119900000000001</v>
+      </c>
+      <c r="E40" s="14">
+        <v>21.105499999999999</v>
+      </c>
+      <c r="F40" s="14">
+        <v>21.1066</v>
+      </c>
+      <c r="G40" s="14">
+        <v>20.709199999999999</v>
+      </c>
+      <c r="H40" s="14">
+        <v>20.716699999999999</v>
+      </c>
+      <c r="I40" s="14">
+        <v>20.709199999999999</v>
+      </c>
+      <c r="J40" s="14">
+        <v>20.716699999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="12"/>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -1987,29 +2006,29 @@
       <c r="C41" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="4">
-        <v>32.485999999999997</v>
-      </c>
-      <c r="E41" s="4">
-        <v>13.7882</v>
-      </c>
-      <c r="F41" s="4">
-        <v>14.163399999999999</v>
-      </c>
-      <c r="G41" s="4">
-        <v>5.6036099999999998</v>
-      </c>
-      <c r="H41" s="7">
-        <v>3.97716</v>
-      </c>
-      <c r="I41" s="7">
-        <v>8.7979099999999999</v>
-      </c>
-      <c r="J41" s="7">
-        <v>7.1407699999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D41" s="14">
+        <v>63.948</v>
+      </c>
+      <c r="E41" s="15">
+        <v>5.7019800000000002E-2</v>
+      </c>
+      <c r="F41" s="14">
+        <v>8.3760299999999996E-2</v>
+      </c>
+      <c r="G41" s="14">
+        <v>9.8660600000000001E-2</v>
+      </c>
+      <c r="H41" s="14">
+        <v>5.0851800000000003E-2</v>
+      </c>
+      <c r="I41" s="14">
+        <v>9.8660600000000001E-2</v>
+      </c>
+      <c r="J41" s="14">
+        <v>5.0851800000000003E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="12"/>
       <c r="B42" s="3" t="s">
         <v>6</v>
@@ -2017,29 +2036,29 @@
       <c r="C42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="6">
-        <v>0.27936899999999998</v>
-      </c>
-      <c r="E42" s="4">
-        <v>1.74153E-17</v>
-      </c>
-      <c r="F42" s="4">
-        <v>4.0991200000000002E-15</v>
-      </c>
-      <c r="G42" s="4">
-        <v>0</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1.95922E-17</v>
-      </c>
-      <c r="I42" s="4">
-        <v>0</v>
-      </c>
-      <c r="J42" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D42" s="14">
+        <v>1.6959</v>
+      </c>
+      <c r="E42" s="14">
+        <v>1.08647E-8</v>
+      </c>
+      <c r="F42" s="14">
+        <v>1.86584E-10</v>
+      </c>
+      <c r="G42" s="14">
+        <v>1.8147399999999999E-8</v>
+      </c>
+      <c r="H42" s="14">
+        <v>1.20514E-14</v>
+      </c>
+      <c r="I42" s="14">
+        <v>1.8147399999999999E-8</v>
+      </c>
+      <c r="J42" s="14">
+        <v>1.20514E-14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="12"/>
       <c r="B43" s="3" t="s">
         <v>7</v>
@@ -2047,29 +2066,29 @@
       <c r="C43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="6">
-        <v>126.812</v>
-      </c>
-      <c r="E43" s="4">
-        <v>12.1471</v>
-      </c>
-      <c r="F43" s="4">
-        <v>12.186500000000001</v>
-      </c>
-      <c r="G43" s="4">
-        <v>28.178799999999999</v>
-      </c>
-      <c r="H43" s="4">
-        <v>28.884799999999998</v>
-      </c>
-      <c r="I43" s="4">
-        <v>5.4335599999999999E-15</v>
-      </c>
-      <c r="J43" s="5">
-        <v>6.9661100000000001E-16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D43" s="14">
+        <v>302.40300000000002</v>
+      </c>
+      <c r="E43" s="15">
+        <v>235.756</v>
+      </c>
+      <c r="F43" s="14">
+        <v>230.46199999999999</v>
+      </c>
+      <c r="G43" s="14">
+        <v>101.983</v>
+      </c>
+      <c r="H43" s="14">
+        <v>98.814800000000005</v>
+      </c>
+      <c r="I43" s="14">
+        <v>101.983</v>
+      </c>
+      <c r="J43" s="14">
+        <v>98.814800000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="12"/>
       <c r="B44" s="3" t="s">
         <v>8</v>
@@ -2077,29 +2096,29 @@
       <c r="C44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="6">
-        <v>195.85400000000001</v>
-      </c>
-      <c r="E44" s="4">
-        <v>61.351399999999998</v>
-      </c>
-      <c r="F44" s="4">
-        <v>64.094099999999997</v>
-      </c>
-      <c r="G44" s="4">
-        <v>77.900899999999993</v>
-      </c>
-      <c r="H44" s="4">
-        <v>78.036600000000007</v>
-      </c>
-      <c r="I44" s="4">
-        <v>18.2437</v>
-      </c>
-      <c r="J44" s="7">
-        <v>18.7578</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D44" s="14">
+        <v>419.43099999999998</v>
+      </c>
+      <c r="E44" s="14">
+        <v>298.56400000000002</v>
+      </c>
+      <c r="F44" s="14">
+        <v>299.80700000000002</v>
+      </c>
+      <c r="G44" s="14">
+        <v>211.25</v>
+      </c>
+      <c r="H44" s="14">
+        <v>212.14500000000001</v>
+      </c>
+      <c r="I44" s="14">
+        <v>211.25</v>
+      </c>
+      <c r="J44" s="14">
+        <v>212.14500000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="12"/>
       <c r="B45" s="3" t="s">
         <v>9</v>
@@ -2107,29 +2126,29 @@
       <c r="C45" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="6">
-        <v>4559.67</v>
-      </c>
-      <c r="E45" s="4">
-        <v>407.09100000000001</v>
-      </c>
-      <c r="F45" s="4">
-        <v>406.67399999999998</v>
-      </c>
-      <c r="G45" s="4">
-        <v>965.64</v>
-      </c>
-      <c r="H45" s="4">
-        <v>990.35900000000004</v>
-      </c>
-      <c r="I45" s="4">
-        <v>4.7009699999999999</v>
-      </c>
-      <c r="J45" s="5">
-        <v>3.41147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D45" s="14">
+        <v>10221.299999999999</v>
+      </c>
+      <c r="E45" s="15">
+        <v>9607.26</v>
+      </c>
+      <c r="F45" s="14">
+        <v>9373.67</v>
+      </c>
+      <c r="G45" s="14">
+        <v>4189.3599999999997</v>
+      </c>
+      <c r="H45" s="14">
+        <v>4107.22</v>
+      </c>
+      <c r="I45" s="14">
+        <v>4189.3599999999997</v>
+      </c>
+      <c r="J45" s="14">
+        <v>4107.22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="12"/>
       <c r="B46" s="3" t="s">
         <v>10</v>
@@ -2137,29 +2156,29 @@
       <c r="C46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="4">
-        <v>6639.53</v>
-      </c>
-      <c r="E46" s="4">
-        <v>3501.42</v>
-      </c>
-      <c r="F46" s="4">
-        <v>3510.21</v>
-      </c>
-      <c r="G46" s="4">
-        <v>3898.56</v>
-      </c>
-      <c r="H46" s="4">
-        <v>3837.16</v>
-      </c>
-      <c r="I46" s="4">
-        <v>1394.56</v>
-      </c>
-      <c r="J46" s="7">
-        <v>1329.44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D46" s="14">
+        <v>13129.6</v>
+      </c>
+      <c r="E46" s="14">
+        <v>12420</v>
+      </c>
+      <c r="F46" s="14">
+        <v>12417</v>
+      </c>
+      <c r="G46" s="14">
+        <v>9026.8700000000008</v>
+      </c>
+      <c r="H46" s="14">
+        <v>9018.2099999999991</v>
+      </c>
+      <c r="I46" s="14">
+        <v>9026.8700000000008</v>
+      </c>
+      <c r="J46" s="14">
+        <v>9018.2099999999991</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="12"/>
       <c r="B47" s="3" t="s">
         <v>11</v>
@@ -2167,29 +2186,29 @@
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="4">
-        <v>2.1954400000000001</v>
-      </c>
-      <c r="E47" s="4">
-        <v>0.69625899999999996</v>
-      </c>
-      <c r="F47" s="4">
-        <v>0.69176899999999997</v>
-      </c>
-      <c r="G47" s="4">
-        <v>0.76464500000000002</v>
-      </c>
-      <c r="H47" s="4">
-        <v>0.769038</v>
-      </c>
-      <c r="I47" s="4">
-        <v>0.18904399999999999</v>
-      </c>
-      <c r="J47" s="7">
-        <v>0.18802099999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D47" s="14">
+        <v>3.1376900000000001</v>
+      </c>
+      <c r="E47" s="14">
+        <v>3.0333899999999998</v>
+      </c>
+      <c r="F47" s="14">
+        <v>3.0444</v>
+      </c>
+      <c r="G47" s="14">
+        <v>1.1562600000000001</v>
+      </c>
+      <c r="H47" s="14">
+        <v>1.1542300000000001</v>
+      </c>
+      <c r="I47" s="14">
+        <v>1.1562600000000001</v>
+      </c>
+      <c r="J47" s="14">
+        <v>1.1542300000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="12"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -2197,29 +2216,29 @@
       <c r="C48" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="4">
-        <v>0.44996700000000001</v>
-      </c>
-      <c r="E48" s="4">
-        <v>0.21293899999999999</v>
-      </c>
-      <c r="F48" s="4">
-        <v>0.22465199999999999</v>
-      </c>
-      <c r="G48" s="4">
-        <v>0.21718799999999999</v>
-      </c>
-      <c r="H48" s="4">
-        <v>0.228406</v>
-      </c>
-      <c r="I48" s="4">
-        <v>0.15492300000000001</v>
-      </c>
-      <c r="J48" s="7">
-        <v>0.17369399999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D48" s="14">
+        <v>0.62943300000000002</v>
+      </c>
+      <c r="E48" s="14">
+        <v>0.34206500000000001</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.34546700000000002</v>
+      </c>
+      <c r="G48" s="14">
+        <v>0.33516600000000002</v>
+      </c>
+      <c r="H48" s="14">
+        <v>0.32486100000000001</v>
+      </c>
+      <c r="I48" s="14">
+        <v>0.33516600000000002</v>
+      </c>
+      <c r="J48" s="14">
+        <v>0.32486100000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="12"/>
       <c r="B49" s="3" t="s">
         <v>19</v>
@@ -2227,29 +2246,29 @@
       <c r="C49" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="4">
-        <v>0.278949</v>
-      </c>
-      <c r="E49" s="4">
-        <v>0.236981</v>
-      </c>
-      <c r="F49" s="4">
-        <v>0.23897699999999999</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0.227384</v>
-      </c>
-      <c r="H49" s="4">
-        <v>0.247251</v>
-      </c>
-      <c r="I49" s="4">
-        <v>0.21333299999999999</v>
-      </c>
-      <c r="J49" s="4">
-        <v>0.22914300000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D49" s="14">
+        <v>0.32250699999999999</v>
+      </c>
+      <c r="E49" s="14">
+        <v>0.32635500000000001</v>
+      </c>
+      <c r="F49" s="14">
+        <v>0.32902399999999998</v>
+      </c>
+      <c r="G49" s="14">
+        <v>0.307089</v>
+      </c>
+      <c r="H49" s="14">
+        <v>0.30938500000000002</v>
+      </c>
+      <c r="I49" s="14">
+        <v>0.307089</v>
+      </c>
+      <c r="J49" s="14">
+        <v>0.30938500000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="12"/>
       <c r="B50" s="3" t="s">
         <v>20</v>
@@ -2257,29 +2276,29 @@
       <c r="C50" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D50" s="6">
-        <v>18.3794</v>
-      </c>
-      <c r="E50" s="4">
-        <v>6.9556100000000001</v>
-      </c>
-      <c r="F50" s="4">
-        <v>7.0234199999999998</v>
-      </c>
-      <c r="G50" s="4">
-        <v>8.9435000000000002</v>
-      </c>
-      <c r="H50" s="4">
-        <v>9.0207599999999992</v>
-      </c>
-      <c r="I50" s="4">
-        <v>2.4412099999999999</v>
-      </c>
-      <c r="J50" s="7">
-        <v>2.5117400000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D50" s="14">
+        <v>99.903999999999996</v>
+      </c>
+      <c r="E50" s="14">
+        <v>27.309799999999999</v>
+      </c>
+      <c r="F50" s="14">
+        <v>27.6738</v>
+      </c>
+      <c r="G50" s="14">
+        <v>23.697800000000001</v>
+      </c>
+      <c r="H50" s="14">
+        <v>23.622199999999999</v>
+      </c>
+      <c r="I50" s="14">
+        <v>23.697800000000001</v>
+      </c>
+      <c r="J50" s="14">
+        <v>23.622199999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="12"/>
       <c r="B51" s="3" t="s">
         <v>21</v>
@@ -2287,29 +2306,29 @@
       <c r="C51" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="4">
-        <v>12.6866</v>
-      </c>
-      <c r="E51" s="4">
-        <v>10.717000000000001</v>
-      </c>
-      <c r="F51" s="4">
-        <v>10.689399999999999</v>
-      </c>
-      <c r="G51" s="4">
-        <v>11.003500000000001</v>
-      </c>
-      <c r="H51" s="4">
-        <v>10.989000000000001</v>
-      </c>
-      <c r="I51" s="4">
-        <v>9.1163100000000004</v>
-      </c>
-      <c r="J51" s="4">
-        <v>9.0694300000000005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D51" s="14">
+        <v>22.512899999999998</v>
+      </c>
+      <c r="E51" s="14">
+        <v>21.985499999999998</v>
+      </c>
+      <c r="F51" s="14">
+        <v>21.970400000000001</v>
+      </c>
+      <c r="G51" s="14">
+        <v>20.486899999999999</v>
+      </c>
+      <c r="H51" s="14">
+        <v>20.527699999999999</v>
+      </c>
+      <c r="I51" s="14">
+        <v>20.486899999999999</v>
+      </c>
+      <c r="J51" s="14">
+        <v>20.527699999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="11" t="s">
         <v>38</v>
       </c>
@@ -2319,29 +2338,29 @@
       <c r="C52" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="6">
-        <v>3701300</v>
-      </c>
-      <c r="E52" s="4">
-        <v>267.05500000000001</v>
-      </c>
-      <c r="F52" s="7">
-        <v>296.529</v>
-      </c>
-      <c r="G52" s="4">
-        <v>406.94299999999998</v>
-      </c>
-      <c r="H52" s="4">
-        <v>383.846</v>
-      </c>
-      <c r="I52" s="4">
-        <v>247.35499999999999</v>
-      </c>
-      <c r="J52" s="4">
-        <v>420.99900000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D52" s="14">
+        <v>26300700</v>
+      </c>
+      <c r="E52" s="14">
+        <v>1093070</v>
+      </c>
+      <c r="F52" s="14">
+        <v>1171340</v>
+      </c>
+      <c r="G52" s="14">
+        <v>2091.34</v>
+      </c>
+      <c r="H52" s="14">
+        <v>2335.0700000000002</v>
+      </c>
+      <c r="I52" s="14">
+        <v>2091.34</v>
+      </c>
+      <c r="J52" s="14">
+        <v>2335.0700000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="12"/>
       <c r="B53" s="3" t="s">
         <v>23</v>
@@ -2349,29 +2368,29 @@
       <c r="C53" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D53" s="6">
-        <v>165480</v>
-      </c>
-      <c r="E53" s="4">
-        <v>21.988099999999999</v>
-      </c>
-      <c r="F53" s="4">
-        <v>20.677</v>
-      </c>
-      <c r="G53" s="4">
-        <v>38.487099999999998</v>
-      </c>
-      <c r="H53" s="4">
-        <v>40.285899999999998</v>
-      </c>
-      <c r="I53" s="4">
-        <v>9.1368200000000002</v>
-      </c>
-      <c r="J53" s="7">
-        <v>16.4497</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D53" s="14">
+        <v>329377</v>
+      </c>
+      <c r="E53" s="14">
+        <v>1821.69</v>
+      </c>
+      <c r="F53" s="14">
+        <v>1943.54</v>
+      </c>
+      <c r="G53" s="14">
+        <v>90.987399999999994</v>
+      </c>
+      <c r="H53" s="14">
+        <v>83.1143</v>
+      </c>
+      <c r="I53" s="14">
+        <v>90.987399999999994</v>
+      </c>
+      <c r="J53" s="14">
+        <v>83.1143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="12"/>
       <c r="B54" s="3" t="s">
         <v>24</v>
@@ -2379,29 +2398,29 @@
       <c r="C54" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="4">
-        <v>11.8787</v>
-      </c>
-      <c r="E54" s="4">
-        <v>5.0997899999999996</v>
-      </c>
-      <c r="F54" s="4">
-        <v>4.8965300000000003</v>
-      </c>
-      <c r="G54" s="4">
-        <v>5.2138999999999998</v>
-      </c>
-      <c r="H54" s="4">
-        <v>5.2250199999999998</v>
-      </c>
-      <c r="I54" s="4">
-        <v>3.60175</v>
-      </c>
-      <c r="J54" s="7">
-        <v>4.0993399999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D54" s="14">
+        <v>51.5381</v>
+      </c>
+      <c r="E54" s="14">
+        <v>35.552100000000003</v>
+      </c>
+      <c r="F54" s="14">
+        <v>16.146599999999999</v>
+      </c>
+      <c r="G54" s="14">
+        <v>32.939300000000003</v>
+      </c>
+      <c r="H54" s="14">
+        <v>19.7179</v>
+      </c>
+      <c r="I54" s="14">
+        <v>32.939300000000003</v>
+      </c>
+      <c r="J54" s="14">
+        <v>19.7179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="12"/>
       <c r="B55" s="3" t="s">
         <v>25</v>
@@ -2409,29 +2428,29 @@
       <c r="C55" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D55" s="4">
-        <v>4343.1000000000004</v>
-      </c>
-      <c r="E55" s="4">
-        <v>291.53199999999998</v>
-      </c>
-      <c r="F55" s="4">
-        <v>1644.22</v>
-      </c>
-      <c r="G55" s="4">
-        <v>24.012</v>
-      </c>
-      <c r="H55" s="4">
-        <v>23.332599999999999</v>
-      </c>
-      <c r="I55" s="4">
-        <v>4.8087799999999996</v>
-      </c>
-      <c r="J55" s="5">
-        <v>3.8368699999999998</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D55" s="14">
+        <v>53551</v>
+      </c>
+      <c r="E55" s="14">
+        <v>5829.06</v>
+      </c>
+      <c r="F55" s="14">
+        <v>5913.2</v>
+      </c>
+      <c r="G55" s="14">
+        <v>79.064999999999998</v>
+      </c>
+      <c r="H55" s="14">
+        <v>74.525499999999994</v>
+      </c>
+      <c r="I55" s="14">
+        <v>79.064999999999998</v>
+      </c>
+      <c r="J55" s="14">
+        <v>74.525499999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="12"/>
       <c r="B56" s="3" t="s">
         <v>26</v>
@@ -2439,29 +2458,29 @@
       <c r="C56" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D56" s="6">
-        <v>521494</v>
-      </c>
-      <c r="E56" s="4">
-        <v>337.59199999999998</v>
-      </c>
-      <c r="F56" s="4">
-        <v>341.53899999999999</v>
-      </c>
-      <c r="G56" s="4">
-        <v>464.964</v>
-      </c>
-      <c r="H56" s="4">
-        <v>504.87299999999999</v>
-      </c>
-      <c r="I56" s="4">
-        <v>112.26600000000001</v>
-      </c>
-      <c r="J56" s="7">
-        <v>160.947</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D56" s="14">
+        <v>10691800</v>
+      </c>
+      <c r="E56" s="14">
+        <v>688467</v>
+      </c>
+      <c r="F56" s="14">
+        <v>709572</v>
+      </c>
+      <c r="G56" s="14">
+        <v>661.95399999999995</v>
+      </c>
+      <c r="H56" s="14">
+        <v>886.68600000000004</v>
+      </c>
+      <c r="I56" s="14">
+        <v>661.95399999999995</v>
+      </c>
+      <c r="J56" s="14">
+        <v>886.68600000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="12"/>
       <c r="B57" s="3" t="s">
         <v>27</v>
@@ -2469,29 +2488,29 @@
       <c r="C57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="4">
-        <v>322.58100000000002</v>
-      </c>
-      <c r="E57" s="4">
-        <v>205.779</v>
-      </c>
-      <c r="F57" s="4">
-        <v>194.852</v>
-      </c>
-      <c r="G57" s="4">
-        <v>182.31800000000001</v>
-      </c>
-      <c r="H57" s="4">
-        <v>178.47900000000001</v>
-      </c>
-      <c r="I57" s="4">
-        <v>48.537399999999998</v>
-      </c>
-      <c r="J57" s="7">
-        <v>55.078099999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D57" s="14">
+        <v>1335.35</v>
+      </c>
+      <c r="E57" s="14">
+        <v>960.03200000000004</v>
+      </c>
+      <c r="F57" s="14">
+        <v>947.04700000000003</v>
+      </c>
+      <c r="G57" s="14">
+        <v>793.63199999999995</v>
+      </c>
+      <c r="H57" s="16">
+        <v>763.90800000000002</v>
+      </c>
+      <c r="I57" s="14">
+        <v>793.63199999999995</v>
+      </c>
+      <c r="J57" s="14">
+        <v>763.90800000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="11" t="s">
         <v>39</v>
       </c>
@@ -2501,29 +2520,29 @@
       <c r="C58" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D58" s="4">
-        <v>315.392</v>
-      </c>
-      <c r="E58" s="4">
-        <v>315.24400000000003</v>
-      </c>
-      <c r="F58" s="4">
-        <v>315.24400000000003</v>
-      </c>
-      <c r="G58" s="4">
-        <v>315.24400000000003</v>
-      </c>
-      <c r="H58" s="4">
-        <v>315.24400000000003</v>
-      </c>
-      <c r="I58" s="4">
-        <v>315.24400000000003</v>
-      </c>
-      <c r="J58" s="4">
-        <v>315.24400000000003</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D58" s="14">
+        <v>328.93200000000002</v>
+      </c>
+      <c r="E58" s="14">
+        <v>326.63400000000001</v>
+      </c>
+      <c r="F58" s="14">
+        <v>326.63400000000001</v>
+      </c>
+      <c r="G58" s="14">
+        <v>326.63400000000001</v>
+      </c>
+      <c r="H58" s="14">
+        <v>326.63400000000001</v>
+      </c>
+      <c r="I58" s="14">
+        <v>326.63400000000001</v>
+      </c>
+      <c r="J58" s="14">
+        <v>326.63400000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="12"/>
       <c r="B59" s="3" t="s">
         <v>29</v>
@@ -2531,29 +2550,29 @@
       <c r="C59" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D59" s="4">
-        <v>227.26</v>
-      </c>
-      <c r="E59" s="4">
-        <v>223.59299999999999</v>
-      </c>
-      <c r="F59" s="4">
-        <v>223.49</v>
-      </c>
-      <c r="G59" s="4">
-        <v>223.59899999999999</v>
-      </c>
-      <c r="H59" s="4">
-        <v>223.59</v>
-      </c>
-      <c r="I59" s="4">
-        <v>223.93899999999999</v>
-      </c>
-      <c r="J59" s="4">
-        <v>223.58099999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D59" s="14">
+        <v>204.09</v>
+      </c>
+      <c r="E59" s="14">
+        <v>202.88300000000001</v>
+      </c>
+      <c r="F59" s="14">
+        <v>202.81200000000001</v>
+      </c>
+      <c r="G59" s="14">
+        <v>202.94399999999999</v>
+      </c>
+      <c r="H59" s="14">
+        <v>202.82599999999999</v>
+      </c>
+      <c r="I59" s="14">
+        <v>202.94399999999999</v>
+      </c>
+      <c r="J59" s="14">
+        <v>202.82599999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="12"/>
       <c r="B60" s="3" t="s">
         <v>30</v>
@@ -2561,29 +2580,29 @@
       <c r="C60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D60" s="4">
-        <v>230.131</v>
-      </c>
-      <c r="E60" s="4">
-        <v>202.98599999999999</v>
-      </c>
-      <c r="F60" s="4">
-        <v>202.78</v>
-      </c>
-      <c r="G60" s="4">
-        <v>203.923</v>
-      </c>
-      <c r="H60" s="4">
-        <v>203.285</v>
-      </c>
-      <c r="I60" s="4">
-        <v>202.66</v>
-      </c>
-      <c r="J60" s="4">
-        <v>202.63399999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D60" s="14">
+        <v>277.41000000000003</v>
+      </c>
+      <c r="E60" s="14">
+        <v>200.32499999999999</v>
+      </c>
+      <c r="F60" s="14">
+        <v>200.84800000000001</v>
+      </c>
+      <c r="G60" s="14">
+        <v>200.411</v>
+      </c>
+      <c r="H60" s="14">
+        <v>200.28200000000001</v>
+      </c>
+      <c r="I60" s="14">
+        <v>200.411</v>
+      </c>
+      <c r="J60" s="14">
+        <v>200.28200000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="12"/>
       <c r="B61" s="3" t="s">
         <v>31</v>
@@ -2591,29 +2610,29 @@
       <c r="C61" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D61" s="4">
-        <v>100.449</v>
-      </c>
-      <c r="E61" s="4">
-        <v>100.23699999999999</v>
-      </c>
-      <c r="F61" s="4">
-        <v>100.241</v>
-      </c>
-      <c r="G61" s="4">
-        <v>100.23099999999999</v>
-      </c>
-      <c r="H61" s="4">
-        <v>100.233</v>
-      </c>
-      <c r="I61" s="4">
-        <v>100.154</v>
-      </c>
-      <c r="J61" s="4">
-        <v>100.15900000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D61" s="14">
+        <v>100.629</v>
+      </c>
+      <c r="E61" s="14">
+        <v>105.006</v>
+      </c>
+      <c r="F61" s="14">
+        <v>114.072</v>
+      </c>
+      <c r="G61" s="14">
+        <v>119.887</v>
+      </c>
+      <c r="H61" s="14">
+        <v>125.78</v>
+      </c>
+      <c r="I61" s="14">
+        <v>119.887</v>
+      </c>
+      <c r="J61" s="14">
+        <v>125.78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="12"/>
       <c r="B62" s="3" t="s">
         <v>32</v>
@@ -2621,29 +2640,29 @@
       <c r="C62" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D62" s="4">
-        <v>592.82799999999997</v>
-      </c>
-      <c r="E62" s="4">
-        <v>313.06299999999999</v>
-      </c>
-      <c r="F62" s="4">
-        <v>311.358</v>
-      </c>
-      <c r="G62" s="4">
-        <v>330.34100000000001</v>
-      </c>
-      <c r="H62" s="4">
-        <v>304.38799999999998</v>
-      </c>
-      <c r="I62" s="4">
-        <v>319.98099999999999</v>
-      </c>
-      <c r="J62" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D62" s="14">
+        <v>1335.66</v>
+      </c>
+      <c r="E62" s="14">
+        <v>422.56200000000001</v>
+      </c>
+      <c r="F62" s="14">
+        <v>415.55799999999999</v>
+      </c>
+      <c r="G62" s="14">
+        <v>401.24599999999998</v>
+      </c>
+      <c r="H62" s="14">
+        <v>401.803</v>
+      </c>
+      <c r="I62" s="14">
+        <v>401.24599999999998</v>
+      </c>
+      <c r="J62" s="14">
+        <v>401.803</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="12"/>
       <c r="B63" s="3" t="s">
         <v>33</v>
@@ -2651,29 +2670,29 @@
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="4">
-        <v>1005.76</v>
-      </c>
-      <c r="E63" s="4">
-        <v>826.81100000000004</v>
-      </c>
-      <c r="F63" s="4">
-        <v>821.92399999999998</v>
-      </c>
-      <c r="G63" s="4">
-        <v>833.69600000000003</v>
-      </c>
-      <c r="H63" s="4">
-        <v>806.755</v>
-      </c>
-      <c r="I63" s="4">
-        <v>802.56799999999998</v>
-      </c>
-      <c r="J63" s="4">
-        <v>800.97199999999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D63" s="14">
+        <v>1326.7</v>
+      </c>
+      <c r="E63" s="14">
+        <v>474.11099999999999</v>
+      </c>
+      <c r="F63" s="14">
+        <v>475.97500000000002</v>
+      </c>
+      <c r="G63" s="14">
+        <v>482.16500000000002</v>
+      </c>
+      <c r="H63" s="14">
+        <v>477.28899999999999</v>
+      </c>
+      <c r="I63" s="14">
+        <v>482.16500000000002</v>
+      </c>
+      <c r="J63" s="14">
+        <v>477.28899999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="12"/>
       <c r="B64" s="3" t="s">
         <v>34</v>
@@ -2681,29 +2700,29 @@
       <c r="C64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="6">
-        <v>21109.5</v>
-      </c>
-      <c r="E64" s="4">
-        <v>716.07299999999998</v>
-      </c>
-      <c r="F64" s="4">
-        <v>717.495</v>
-      </c>
-      <c r="G64" s="4">
-        <v>716.72900000000004</v>
-      </c>
-      <c r="H64" s="4">
-        <v>717.16600000000005</v>
-      </c>
-      <c r="I64" s="4">
-        <v>708.88</v>
-      </c>
-      <c r="J64" s="4">
-        <v>717.27800000000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D64" s="14">
+        <v>328446</v>
+      </c>
+      <c r="E64" s="14">
+        <v>44533.8</v>
+      </c>
+      <c r="F64" s="14">
+        <v>50368.2</v>
+      </c>
+      <c r="G64" s="14">
+        <v>1058.77</v>
+      </c>
+      <c r="H64" s="14">
+        <v>1157.3800000000001</v>
+      </c>
+      <c r="I64" s="14">
+        <v>1058.77</v>
+      </c>
+      <c r="J64" s="14">
+        <v>1157.3800000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="12"/>
       <c r="B65" s="3" t="s">
         <v>35</v>
@@ -2711,30 +2730,1160 @@
       <c r="C65" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="6">
-        <v>11050.8</v>
-      </c>
-      <c r="E65" s="4">
-        <v>863.64</v>
-      </c>
-      <c r="F65" s="4">
-        <v>1060.58</v>
-      </c>
-      <c r="G65" s="4">
-        <v>1156.8900000000001</v>
-      </c>
-      <c r="H65" s="4">
-        <v>1272.58</v>
-      </c>
-      <c r="I65" s="7">
-        <v>706.89800000000002</v>
-      </c>
-      <c r="J65" s="4">
-        <v>1619.65</v>
-      </c>
+      <c r="D65" s="14">
+        <v>158276</v>
+      </c>
+      <c r="E65" s="14">
+        <v>7293.89</v>
+      </c>
+      <c r="F65" s="14">
+        <v>8127.22</v>
+      </c>
+      <c r="G65" s="14">
+        <v>4581.91</v>
+      </c>
+      <c r="H65" s="14">
+        <v>4988.22</v>
+      </c>
+      <c r="I65" s="14">
+        <v>4581.91</v>
+      </c>
+      <c r="J65" s="14">
+        <v>4988.22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="18">
+      <c r="A67" s="3"/>
+      <c r="B67" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="14">
+        <v>3437090000</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="12"/>
+      <c r="B70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="14">
+        <v>22292400000</v>
+      </c>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="12"/>
+      <c r="B71" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="14">
+        <v>471270</v>
+      </c>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="14">
+        <v>2989.19</v>
+      </c>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="12"/>
+      <c r="B73" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" s="14">
+        <v>21.3184</v>
+      </c>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="12"/>
+      <c r="B74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="14">
+        <v>149.59800000000001</v>
+      </c>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="12"/>
+      <c r="B75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="14">
+        <v>148.22499999999999</v>
+      </c>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="12"/>
+      <c r="B76" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="14">
+        <v>847.10599999999999</v>
+      </c>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="12"/>
+      <c r="B77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="14">
+        <v>1061.67</v>
+      </c>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="12"/>
+      <c r="B78" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" s="14">
+        <v>25971</v>
+      </c>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="12"/>
+      <c r="B79" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="14">
+        <v>30281.7</v>
+      </c>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="12"/>
+      <c r="B80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D80" s="14">
+        <v>3.9605199999999998</v>
+      </c>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="12"/>
+      <c r="B81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="14">
+        <v>0.82067900000000005</v>
+      </c>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="12"/>
+      <c r="B82" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D82" s="14">
+        <v>42.122199999999999</v>
+      </c>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="12"/>
+      <c r="B83" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D83" s="14">
+        <v>197945</v>
+      </c>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="12"/>
+      <c r="B84" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D84" s="14">
+        <v>46.834699999999998</v>
+      </c>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D85" s="14">
+        <v>272670000</v>
+      </c>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="12"/>
+      <c r="B86" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="14">
+        <v>163485</v>
+      </c>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="12"/>
+      <c r="B87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D87" s="14">
+        <v>146.99100000000001</v>
+      </c>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="12"/>
+      <c r="B88" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D88" s="14">
+        <v>275040</v>
+      </c>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="12"/>
+      <c r="B89" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" s="14">
+        <v>120429000</v>
+      </c>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="12"/>
+      <c r="B90" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D90" s="14">
+        <v>4245.38</v>
+      </c>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D91" s="14">
+        <v>454.31099999999998</v>
+      </c>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="12"/>
+      <c r="B92" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D92" s="14">
+        <v>569.83399999999995</v>
+      </c>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="12"/>
+      <c r="B93" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D93" s="14">
+        <v>700.90599999999995</v>
+      </c>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="12"/>
+      <c r="B94" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D94" s="14">
+        <v>304.92899999999997</v>
+      </c>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="12"/>
+      <c r="B95" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D95" s="14">
+        <v>3735.44</v>
+      </c>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="12"/>
+      <c r="B96" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D96" s="14">
+        <v>3533.33</v>
+      </c>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="12"/>
+      <c r="B97" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D97" s="14">
+        <v>857154</v>
+      </c>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="12"/>
+      <c r="B98" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D98" s="14">
+        <v>2598680</v>
+      </c>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+    </row>
+    <row r="100" spans="1:10" ht="18">
+      <c r="A100" s="3"/>
+      <c r="B100" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="14"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="12"/>
+      <c r="B103" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="14"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="12"/>
+      <c r="B104" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="14"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="14"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="12"/>
+      <c r="B106" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="14"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="12"/>
+      <c r="B107" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="14"/>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="12"/>
+      <c r="B108" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="14"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="12"/>
+      <c r="B109" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="14"/>
+      <c r="I109" s="14"/>
+      <c r="J109" s="14"/>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="12"/>
+      <c r="B110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="14"/>
+      <c r="J110" s="14"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="12"/>
+      <c r="B111" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="14"/>
+      <c r="J111" s="14"/>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="12"/>
+      <c r="B112" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
+      <c r="J112" s="14"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="12"/>
+      <c r="B113" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="14"/>
+      <c r="I113" s="14"/>
+      <c r="J113" s="14"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="12"/>
+      <c r="B114" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="14"/>
+      <c r="I114" s="14"/>
+      <c r="J114" s="14"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="12"/>
+      <c r="B115" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="14"/>
+      <c r="I115" s="14"/>
+      <c r="J115" s="14"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="12"/>
+      <c r="B116" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14"/>
+      <c r="I116" s="14"/>
+      <c r="J116" s="14"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="12"/>
+      <c r="B117" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+      <c r="J117" s="14"/>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="14"/>
+      <c r="I118" s="14"/>
+      <c r="J118" s="14"/>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="12"/>
+      <c r="B119" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="14"/>
+      <c r="H119" s="14"/>
+      <c r="I119" s="14"/>
+      <c r="J119" s="14"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="12"/>
+      <c r="B120" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
+      <c r="J120" s="14"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="12"/>
+      <c r="B121" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14"/>
+      <c r="I121" s="14"/>
+      <c r="J121" s="14"/>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="12"/>
+      <c r="B122" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="14"/>
+      <c r="H122" s="14"/>
+      <c r="I122" s="14"/>
+      <c r="J122" s="14"/>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" s="12"/>
+      <c r="B123" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="14"/>
+      <c r="I123" s="14"/>
+      <c r="J123" s="14"/>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="14"/>
+      <c r="I124" s="14"/>
+      <c r="J124" s="14"/>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="12"/>
+      <c r="B125" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
+      <c r="I125" s="14"/>
+      <c r="J125" s="14"/>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" s="12"/>
+      <c r="B126" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="14"/>
+      <c r="I126" s="14"/>
+      <c r="J126" s="14"/>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" s="12"/>
+      <c r="B127" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="14"/>
+      <c r="G127" s="14"/>
+      <c r="H127" s="14"/>
+      <c r="I127" s="14"/>
+      <c r="J127" s="14"/>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" s="12"/>
+      <c r="B128" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
+      <c r="F128" s="14"/>
+      <c r="G128" s="14"/>
+      <c r="H128" s="14"/>
+      <c r="I128" s="14"/>
+      <c r="J128" s="14"/>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="12"/>
+      <c r="B129" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+      <c r="F129" s="14"/>
+      <c r="G129" s="14"/>
+      <c r="H129" s="14"/>
+      <c r="I129" s="14"/>
+      <c r="J129" s="14"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="12"/>
+      <c r="B130" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
+      <c r="F130" s="14"/>
+      <c r="G130" s="14"/>
+      <c r="H130" s="14"/>
+      <c r="I130" s="14"/>
+      <c r="J130" s="14"/>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="A131" s="12"/>
+      <c r="B131" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D131" s="14"/>
+      <c r="E131" s="14"/>
+      <c r="F131" s="14"/>
+      <c r="G131" s="14"/>
+      <c r="H131" s="14"/>
+      <c r="I131" s="14"/>
+      <c r="J131" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="20">
+    <mergeCell ref="B100:J100"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="A105:A117"/>
+    <mergeCell ref="A118:A123"/>
+    <mergeCell ref="A124:A131"/>
+    <mergeCell ref="B67:J67"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A84"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="A91:A98"/>
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A51"/>
@@ -2748,5 +3897,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add iL-SHADE and rectify fileoutput about replacing 0 value by 1e-60
</commit_message>
<xml_diff>
--- a/DE_extension_ExperimentResults.xlsx
+++ b/DE_extension_ExperimentResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MyCode\VisualStudio\meta_algo\DE_extension_to_CEC2014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D73EC4E-3833-4791-ABF2-1E4726923E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DFC5BA-6BE2-4B72-AC16-12FD7FECFA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50E21A78-8C48-40D2-9105-B406553DA780}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="81">
   <si>
     <t>f1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -401,6 +401,14 @@
       </rPr>
       <t xml:space="preserve"> PROBLEMS CEC2014 f1– f30, AVERAGED OVER 51 INDEPENDENT RUNS, EVALUATION D*10000 TIMES</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iL-SHADE w/o archive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iL-SHADE with archive</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,7 +476,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,8 +513,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -529,13 +543,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -575,9 +635,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -585,6 +642,54 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -921,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A90AD3-D743-4E65-B2C8-F3B5C98AC2E6}">
-  <dimension ref="A1:M131"/>
+  <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H98" sqref="H98"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -939,26 +1044,29 @@
     <col min="8" max="8" width="25.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.7265625" style="1"/>
-    <col min="13" max="13" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="1"/>
+    <col min="11" max="12" width="28.1796875" style="16" customWidth="1"/>
+    <col min="13" max="14" width="8.7265625" style="1"/>
+    <col min="15" max="15" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="3"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -985,12 +1093,18 @@
       <c r="J2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" s="11" t="s">
         <v>36</v>
       </c>
@@ -1021,12 +1135,18 @@
       <c r="J3" s="5">
         <v>2.8659399999999997E-17</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="3" t="s">
+      <c r="K3" s="13">
+        <v>1.51487E-9</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1.2269E-17</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -1055,12 +1175,18 @@
       <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="3" t="s">
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -1089,8 +1215,14 @@
       <c r="J5" s="5">
         <v>7.8764400000000004E-29</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+      <c r="K5" s="13">
+        <v>6.9595000000000004E-28</v>
+      </c>
+      <c r="L5" s="13">
+        <v>2.3198300000000002E-28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="17" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>37</v>
       </c>
@@ -1121,8 +1253,14 @@
       <c r="J6" s="5">
         <v>4.6460900000000003E-11</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6" s="13">
+        <v>3.8973399999999999E-7</v>
+      </c>
+      <c r="L6" s="13">
+        <v>6.5437799999999999E-17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1151,8 +1289,14 @@
       <c r="J7" s="4">
         <v>20.157499999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="13">
+        <v>20.894600000000001</v>
+      </c>
+      <c r="L7" s="13">
+        <v>20.871400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="12"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -1181,8 +1325,14 @@
       <c r="J8" s="7">
         <v>7.1407699999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="K8" s="13">
+        <v>2.9283400000000001E-7</v>
+      </c>
+      <c r="L8" s="13">
+        <v>3.1391000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -1211,8 +1361,14 @@
       <c r="J9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -1241,8 +1397,14 @@
       <c r="J10" s="5">
         <v>6.9661100000000001E-16</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="K10" s="13">
+        <v>4.4268599999999997E-9</v>
+      </c>
+      <c r="L10" s="13">
+        <v>1.7974600000000001E-12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -1271,8 +1433,14 @@
       <c r="J11" s="7">
         <v>18.7578</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="K11" s="13">
+        <v>9.76084</v>
+      </c>
+      <c r="L11" s="13">
+        <v>9.4226500000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="12"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -1301,8 +1469,14 @@
       <c r="J12" s="5">
         <v>3.41147</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="K12" s="13">
+        <v>7.3311400000000004</v>
+      </c>
+      <c r="L12" s="13">
+        <v>6.21692</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="12"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -1331,8 +1505,14 @@
       <c r="J13" s="7">
         <v>1329.44</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="K13" s="13">
+        <v>1477.28</v>
+      </c>
+      <c r="L13" s="13">
+        <v>1315.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -1361,8 +1541,14 @@
       <c r="J14" s="7">
         <v>0.18802099999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="K14" s="13">
+        <v>0.480628</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0.44831599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="12"/>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -1391,8 +1577,14 @@
       <c r="J15" s="7">
         <v>0.17369399999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="K15" s="13">
+        <v>0.131661</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0.13120100000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
@@ -1421,8 +1613,14 @@
       <c r="J16" s="4">
         <v>0.22914300000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="13">
+        <v>0.22134999999999999</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0.18924099999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="12"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
@@ -1451,8 +1649,14 @@
       <c r="J17" s="7">
         <v>2.5117400000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="13">
+        <v>2.5825300000000002</v>
+      </c>
+      <c r="L17" s="13">
+        <v>2.5043600000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -1481,8 +1685,14 @@
       <c r="J18" s="4">
         <v>9.0694300000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="13">
+        <v>9.1582299999999996</v>
+      </c>
+      <c r="L18" s="13">
+        <v>8.3943999999999992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="11" t="s">
         <v>38</v>
       </c>
@@ -1513,8 +1723,14 @@
       <c r="J19" s="4">
         <v>420.99900000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="13">
+        <v>135.22200000000001</v>
+      </c>
+      <c r="L19" s="13">
+        <v>212.11500000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>23</v>
@@ -1543,8 +1759,14 @@
       <c r="J20" s="7">
         <v>16.4497</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="13">
+        <v>4.3154000000000003</v>
+      </c>
+      <c r="L20" s="13">
+        <v>5.2511099999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="12"/>
       <c r="B21" s="3" t="s">
         <v>24</v>
@@ -1573,8 +1795,14 @@
       <c r="J21" s="7">
         <v>4.0993399999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="13">
+        <v>2.48346</v>
+      </c>
+      <c r="L21" s="13">
+        <v>2.9556399999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="12"/>
       <c r="B22" s="3" t="s">
         <v>25</v>
@@ -1603,8 +1831,14 @@
       <c r="J22" s="5">
         <v>3.8368699999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="13">
+        <v>3.21692</v>
+      </c>
+      <c r="L22" s="13">
+        <v>2.6116600000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="12"/>
       <c r="B23" s="3" t="s">
         <v>26</v>
@@ -1633,8 +1867,14 @@
       <c r="J23" s="7">
         <v>160.947</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="13">
+        <v>73.535700000000006</v>
+      </c>
+      <c r="L23" s="13">
+        <v>77.578100000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
         <v>27</v>
@@ -1663,8 +1903,14 @@
       <c r="J24" s="7">
         <v>55.078099999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" s="13">
+        <v>28.3856</v>
+      </c>
+      <c r="L24" s="13">
+        <v>33.6173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
@@ -1695,8 +1941,14 @@
       <c r="J25" s="4">
         <v>315.24400000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" s="13">
+        <v>289.70100000000002</v>
+      </c>
+      <c r="L25" s="13">
+        <v>289.70100000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
         <v>29</v>
@@ -1725,8 +1977,14 @@
       <c r="J26" s="4">
         <v>223.58099999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="13">
+        <v>200.637</v>
+      </c>
+      <c r="L26" s="13">
+        <v>200.54900000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="12"/>
       <c r="B27" s="3" t="s">
         <v>30</v>
@@ -1755,8 +2013,14 @@
       <c r="J27" s="4">
         <v>202.63399999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="13">
+        <v>206.27600000000001</v>
+      </c>
+      <c r="L27" s="13">
+        <v>206.22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="12"/>
       <c r="B28" s="3" t="s">
         <v>31</v>
@@ -1785,8 +2049,14 @@
       <c r="J28" s="4">
         <v>100.15900000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" s="13">
+        <v>100.13500000000001</v>
+      </c>
+      <c r="L28" s="13">
+        <v>100.129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="12"/>
       <c r="B29" s="3" t="s">
         <v>32</v>
@@ -1815,8 +2085,14 @@
       <c r="J29" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="13">
+        <v>400.07</v>
+      </c>
+      <c r="L29" s="13">
+        <v>392.50299999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="12"/>
       <c r="B30" s="3" t="s">
         <v>33</v>
@@ -1845,8 +2121,14 @@
       <c r="J30" s="4">
         <v>800.97199999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" s="13">
+        <v>408.02499999999998</v>
+      </c>
+      <c r="L30" s="13">
+        <v>407.959</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="12"/>
       <c r="B31" s="3" t="s">
         <v>34</v>
@@ -1875,8 +2157,14 @@
       <c r="J31" s="4">
         <v>717.27800000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" s="13">
+        <v>9526550</v>
+      </c>
+      <c r="L31" s="13">
+        <v>12652800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="12"/>
       <c r="B32" s="3" t="s">
         <v>35</v>
@@ -1905,22 +2193,30 @@
       <c r="J32" s="4">
         <v>1619.65</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="18">
+      <c r="K32" s="13">
+        <v>382.78100000000001</v>
+      </c>
+      <c r="L32" s="13">
+        <v>654.37699999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="18">
       <c r="A34" s="3"/>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="22"/>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
@@ -1947,8 +2243,14 @@
       <c r="J35" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="11" t="s">
         <v>36</v>
       </c>
@@ -1958,29 +2260,35 @@
       <c r="C36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="14">
+      <c r="D36" s="13">
         <v>485320000</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="13">
         <v>6540910</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="13">
         <v>6949670</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>1264920</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="13">
         <v>729528</v>
       </c>
-      <c r="I36" s="14">
+      <c r="I36" s="13">
         <v>1264920</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <v>729528</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36" s="13">
+        <v>6198.79</v>
+      </c>
+      <c r="L36" s="13">
+        <v>1616.32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="12"/>
       <c r="B37" s="3" t="s">
         <v>1</v>
@@ -1988,29 +2296,35 @@
       <c r="C37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="13">
         <v>376403000</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="13">
         <v>3401.12</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F37" s="13">
         <v>3638.82</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>3268.32</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="13">
         <v>94.282399999999996</v>
       </c>
-      <c r="I37" s="14">
+      <c r="I37" s="13">
         <v>3268.32</v>
       </c>
-      <c r="J37" s="14">
+      <c r="J37" s="13">
         <v>94.282399999999996</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" s="13">
+        <v>9.4120000000000007E-13</v>
+      </c>
+      <c r="L37" s="13">
+        <v>3.0157600000000001E-21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="12"/>
       <c r="B38" s="3" t="s">
         <v>2</v>
@@ -2018,29 +2332,35 @@
       <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="13">
         <v>161642</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="13">
         <v>26493.7</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="13">
         <v>25788.6</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <v>2.20017E-7</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="13">
         <v>4.30221E-10</v>
       </c>
-      <c r="I38" s="14">
+      <c r="I38" s="13">
         <v>2.20017E-7</v>
       </c>
-      <c r="J38" s="14">
+      <c r="J38" s="13">
         <v>4.30221E-10</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38" s="13">
+        <v>2.7321099999999999E-17</v>
+      </c>
+      <c r="L38" s="13">
+        <v>7.4405399999999997E-25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="11" t="s">
         <v>37</v>
       </c>
@@ -2050,29 +2370,35 @@
       <c r="C39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="13">
         <v>243.351</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="13">
         <v>96.700299999999999</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="13">
         <v>95.371300000000005</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <v>96.091300000000004</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="13">
         <v>94.047300000000007</v>
       </c>
-      <c r="I39" s="14">
+      <c r="I39" s="13">
         <v>96.091300000000004</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="13">
         <v>94.047300000000007</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39" s="13">
+        <v>30.818100000000001</v>
+      </c>
+      <c r="L39" s="13">
+        <v>57.604300000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="12"/>
       <c r="B40" s="3" t="s">
         <v>4</v>
@@ -2080,29 +2406,35 @@
       <c r="C40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="13">
         <v>21.119900000000001</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="13">
         <v>21.105499999999999</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="13">
         <v>21.1066</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <v>20.709199999999999</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="13">
         <v>20.716699999999999</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="13">
         <v>20.709199999999999</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="13">
         <v>20.716699999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40" s="13">
+        <v>21.1187</v>
+      </c>
+      <c r="L40" s="13">
+        <v>21.092500000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="12"/>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -2110,29 +2442,35 @@
       <c r="C41" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="13">
         <v>63.948</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="14">
         <v>5.7019800000000002E-2</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="13">
         <v>8.3760299999999996E-2</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <v>9.8660600000000001E-2</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="13">
         <v>5.0851800000000003E-2</v>
       </c>
-      <c r="I41" s="14">
+      <c r="I41" s="13">
         <v>9.8660600000000001E-2</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="13">
         <v>5.0851800000000003E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41" s="13">
+        <v>0.11971</v>
+      </c>
+      <c r="L41" s="13">
+        <v>0.121958</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="12"/>
       <c r="B42" s="3" t="s">
         <v>6</v>
@@ -2140,29 +2478,35 @@
       <c r="C42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="13">
         <v>1.6959</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="13">
         <v>1.08647E-8</v>
       </c>
-      <c r="F42" s="14">
+      <c r="F42" s="13">
         <v>1.86584E-10</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="13">
         <v>1.8147399999999999E-8</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="13">
         <v>1.20514E-14</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="13">
         <v>1.8147399999999999E-8</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="13">
         <v>1.20514E-14</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42" s="13">
+        <v>4.3538200000000001E-18</v>
+      </c>
+      <c r="L42" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="12"/>
       <c r="B43" s="3" t="s">
         <v>7</v>
@@ -2170,29 +2514,35 @@
       <c r="C43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="13">
         <v>302.40300000000002</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="14">
         <v>235.756</v>
       </c>
-      <c r="F43" s="14">
+      <c r="F43" s="13">
         <v>230.46199999999999</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="13">
         <v>101.983</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="13">
         <v>98.814800000000005</v>
       </c>
-      <c r="I43" s="14">
+      <c r="I43" s="13">
         <v>101.983</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43" s="13">
         <v>98.814800000000005</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43" s="13">
+        <v>0.65604399999999996</v>
+      </c>
+      <c r="L43" s="13">
+        <v>3.6581199999999999E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="12"/>
       <c r="B44" s="3" t="s">
         <v>8</v>
@@ -2200,29 +2550,35 @@
       <c r="C44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>419.43099999999998</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="13">
         <v>298.56400000000002</v>
       </c>
-      <c r="F44" s="14">
+      <c r="F44" s="13">
         <v>299.80700000000002</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="13">
         <v>211.25</v>
       </c>
-      <c r="H44" s="14">
+      <c r="H44" s="13">
         <v>212.14500000000001</v>
       </c>
-      <c r="I44" s="14">
+      <c r="I44" s="13">
         <v>211.25</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="13">
         <v>212.14500000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44" s="13">
+        <v>22.3245</v>
+      </c>
+      <c r="L44" s="13">
+        <v>18.851700000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="12"/>
       <c r="B45" s="3" t="s">
         <v>9</v>
@@ -2230,29 +2586,35 @@
       <c r="C45" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="13">
         <v>10221.299999999999</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="14">
         <v>9607.26</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="13">
         <v>9373.67</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="13">
         <v>4189.3599999999997</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45" s="13">
         <v>4107.22</v>
       </c>
-      <c r="I45" s="14">
+      <c r="I45" s="13">
         <v>4189.3599999999997</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="13">
         <v>4107.22</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45" s="13">
+        <v>70.547899999999998</v>
+      </c>
+      <c r="L45" s="13">
+        <v>41.944800000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="12"/>
       <c r="B46" s="3" t="s">
         <v>10</v>
@@ -2260,29 +2622,35 @@
       <c r="C46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="13">
         <v>13129.6</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="13">
         <v>12420</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F46" s="13">
         <v>12417</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="13">
         <v>9026.8700000000008</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="13">
         <v>9018.2099999999991</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="13">
         <v>9026.8700000000008</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="13">
         <v>9018.2099999999991</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46" s="13">
+        <v>3922.14</v>
+      </c>
+      <c r="L46" s="13">
+        <v>3605.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="12"/>
       <c r="B47" s="3" t="s">
         <v>11</v>
@@ -2290,29 +2658,35 @@
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="13">
         <v>3.1376900000000001</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="13">
         <v>3.0333899999999998</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="13">
         <v>3.0444</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="13">
         <v>1.1562600000000001</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="13">
         <v>1.1542300000000001</v>
       </c>
-      <c r="I47" s="14">
+      <c r="I47" s="13">
         <v>1.1562600000000001</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="13">
         <v>1.1542300000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47" s="13">
+        <v>0.50511099999999998</v>
+      </c>
+      <c r="L47" s="13">
+        <v>0.55092799999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="12"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -2320,29 +2694,35 @@
       <c r="C48" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="13">
         <v>0.62943300000000002</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="13">
         <v>0.34206500000000001</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="13">
         <v>0.34546700000000002</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="13">
         <v>0.33516600000000002</v>
       </c>
-      <c r="H48" s="14">
+      <c r="H48" s="13">
         <v>0.32486100000000001</v>
       </c>
-      <c r="I48" s="14">
+      <c r="I48" s="13">
         <v>0.33516600000000002</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="13">
         <v>0.32486100000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48" s="13">
+        <v>0.20808299999999999</v>
+      </c>
+      <c r="L48" s="13">
+        <v>0.18254799999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="12"/>
       <c r="B49" s="3" t="s">
         <v>19</v>
@@ -2350,29 +2730,35 @@
       <c r="C49" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="13">
         <v>0.32250699999999999</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="13">
         <v>0.32635500000000001</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="13">
         <v>0.32902399999999998</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="13">
         <v>0.307089</v>
       </c>
-      <c r="H49" s="14">
+      <c r="H49" s="13">
         <v>0.30938500000000002</v>
       </c>
-      <c r="I49" s="14">
+      <c r="I49" s="13">
         <v>0.307089</v>
       </c>
-      <c r="J49" s="14">
+      <c r="J49" s="13">
         <v>0.30938500000000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49" s="13">
+        <v>0.28035500000000002</v>
+      </c>
+      <c r="L49" s="13">
+        <v>0.27732600000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="12"/>
       <c r="B50" s="3" t="s">
         <v>20</v>
@@ -2380,29 +2766,35 @@
       <c r="C50" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="13">
         <v>99.903999999999996</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="13">
         <v>27.309799999999999</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50" s="13">
         <v>27.6738</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G50" s="13">
         <v>23.697800000000001</v>
       </c>
-      <c r="H50" s="14">
+      <c r="H50" s="13">
         <v>23.622199999999999</v>
       </c>
-      <c r="I50" s="14">
+      <c r="I50" s="13">
         <v>23.697800000000001</v>
       </c>
-      <c r="J50" s="14">
+      <c r="J50" s="13">
         <v>23.622199999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50" s="13">
+        <v>6.17469</v>
+      </c>
+      <c r="L50" s="13">
+        <v>6.1230000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="12"/>
       <c r="B51" s="3" t="s">
         <v>21</v>
@@ -2410,29 +2802,35 @@
       <c r="C51" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="13">
         <v>22.512899999999998</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="13">
         <v>21.985499999999998</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="13">
         <v>21.970400000000001</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="13">
         <v>20.486899999999999</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="13">
         <v>20.527699999999999</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="13">
         <v>20.486899999999999</v>
       </c>
-      <c r="J51" s="14">
+      <c r="J51" s="13">
         <v>20.527699999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51" s="13">
+        <v>17.720700000000001</v>
+      </c>
+      <c r="L51" s="13">
+        <v>17.029199999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="11" t="s">
         <v>38</v>
       </c>
@@ -2442,29 +2840,35 @@
       <c r="C52" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="14">
+      <c r="D52" s="13">
         <v>26300700</v>
       </c>
-      <c r="E52" s="14">
+      <c r="E52" s="13">
         <v>1093070</v>
       </c>
-      <c r="F52" s="14">
+      <c r="F52" s="13">
         <v>1171340</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="13">
         <v>2091.34</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="13">
         <v>2335.0700000000002</v>
       </c>
-      <c r="I52" s="14">
+      <c r="I52" s="13">
         <v>2091.34</v>
       </c>
-      <c r="J52" s="14">
+      <c r="J52" s="13">
         <v>2335.0700000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52" s="13">
+        <v>607.75</v>
+      </c>
+      <c r="L52" s="13">
+        <v>1132.5999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="12"/>
       <c r="B53" s="3" t="s">
         <v>23</v>
@@ -2472,29 +2876,35 @@
       <c r="C53" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D53" s="14">
+      <c r="D53" s="13">
         <v>329377</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="13">
         <v>1821.69</v>
       </c>
-      <c r="F53" s="14">
+      <c r="F53" s="13">
         <v>1943.54</v>
       </c>
-      <c r="G53" s="14">
+      <c r="G53" s="13">
         <v>90.987399999999994</v>
       </c>
-      <c r="H53" s="14">
+      <c r="H53" s="13">
         <v>83.1143</v>
       </c>
-      <c r="I53" s="14">
+      <c r="I53" s="13">
         <v>90.987399999999994</v>
       </c>
-      <c r="J53" s="14">
+      <c r="J53" s="13">
         <v>83.1143</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53" s="13">
+        <v>26.037199999999999</v>
+      </c>
+      <c r="L53" s="13">
+        <v>60.789499999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="12"/>
       <c r="B54" s="3" t="s">
         <v>24</v>
@@ -2502,29 +2912,35 @@
       <c r="C54" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="13">
         <v>51.5381</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="13">
         <v>35.552100000000003</v>
       </c>
-      <c r="F54" s="14">
+      <c r="F54" s="13">
         <v>16.146599999999999</v>
       </c>
-      <c r="G54" s="14">
+      <c r="G54" s="13">
         <v>32.939300000000003</v>
       </c>
-      <c r="H54" s="14">
+      <c r="H54" s="13">
         <v>19.7179</v>
       </c>
-      <c r="I54" s="14">
+      <c r="I54" s="13">
         <v>32.939300000000003</v>
       </c>
-      <c r="J54" s="14">
+      <c r="J54" s="13">
         <v>19.7179</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54" s="13">
+        <v>10.240600000000001</v>
+      </c>
+      <c r="L54" s="13">
+        <v>9.2093500000000006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="12"/>
       <c r="B55" s="3" t="s">
         <v>25</v>
@@ -2532,29 +2948,35 @@
       <c r="C55" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D55" s="14">
+      <c r="D55" s="13">
         <v>53551</v>
       </c>
-      <c r="E55" s="14">
+      <c r="E55" s="13">
         <v>5829.06</v>
       </c>
-      <c r="F55" s="14">
+      <c r="F55" s="13">
         <v>5913.2</v>
       </c>
-      <c r="G55" s="14">
+      <c r="G55" s="13">
         <v>79.064999999999998</v>
       </c>
-      <c r="H55" s="14">
+      <c r="H55" s="13">
         <v>74.525499999999994</v>
       </c>
-      <c r="I55" s="14">
+      <c r="I55" s="13">
         <v>79.064999999999998</v>
       </c>
-      <c r="J55" s="14">
+      <c r="J55" s="13">
         <v>74.525499999999994</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55" s="13">
+        <v>11.016</v>
+      </c>
+      <c r="L55" s="13">
+        <v>9.4745899999999992</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="12"/>
       <c r="B56" s="3" t="s">
         <v>26</v>
@@ -2562,29 +2984,35 @@
       <c r="C56" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D56" s="14">
+      <c r="D56" s="13">
         <v>10691800</v>
       </c>
-      <c r="E56" s="14">
+      <c r="E56" s="13">
         <v>688467</v>
       </c>
-      <c r="F56" s="14">
+      <c r="F56" s="13">
         <v>709572</v>
       </c>
-      <c r="G56" s="14">
+      <c r="G56" s="13">
         <v>661.95399999999995</v>
       </c>
-      <c r="H56" s="14">
+      <c r="H56" s="13">
         <v>886.68600000000004</v>
       </c>
-      <c r="I56" s="14">
+      <c r="I56" s="13">
         <v>661.95399999999995</v>
       </c>
-      <c r="J56" s="14">
+      <c r="J56" s="13">
         <v>886.68600000000004</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56" s="13">
+        <v>333.39600000000002</v>
+      </c>
+      <c r="L56" s="13">
+        <v>468.916</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="12"/>
       <c r="B57" s="3" t="s">
         <v>27</v>
@@ -2592,29 +3020,35 @@
       <c r="C57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="14">
+      <c r="D57" s="13">
         <v>1335.35</v>
       </c>
-      <c r="E57" s="14">
+      <c r="E57" s="13">
         <v>960.03200000000004</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="13">
         <v>947.04700000000003</v>
       </c>
-      <c r="G57" s="14">
+      <c r="G57" s="13">
         <v>793.63199999999995</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="15">
         <v>763.90800000000002</v>
       </c>
-      <c r="I57" s="14">
+      <c r="I57" s="13">
         <v>793.63199999999995</v>
       </c>
-      <c r="J57" s="14">
+      <c r="J57" s="13">
         <v>763.90800000000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57" s="13">
+        <v>127.69799999999999</v>
+      </c>
+      <c r="L57" s="13">
+        <v>85.637699999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="11" t="s">
         <v>39</v>
       </c>
@@ -2624,29 +3058,35 @@
       <c r="C58" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D58" s="14">
+      <c r="D58" s="13">
         <v>328.93200000000002</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E58" s="13">
         <v>326.63400000000001</v>
       </c>
-      <c r="F58" s="14">
+      <c r="F58" s="13">
         <v>326.63400000000001</v>
       </c>
-      <c r="G58" s="14">
+      <c r="G58" s="13">
         <v>326.63400000000001</v>
       </c>
-      <c r="H58" s="14">
+      <c r="H58" s="13">
         <v>326.63400000000001</v>
       </c>
-      <c r="I58" s="14">
+      <c r="I58" s="13">
         <v>326.63400000000001</v>
       </c>
-      <c r="J58" s="14">
+      <c r="J58" s="13">
         <v>326.63400000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58" s="13">
+        <v>326.63400000000001</v>
+      </c>
+      <c r="L58" s="13">
+        <v>326.63400000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="12"/>
       <c r="B59" s="3" t="s">
         <v>29</v>
@@ -2654,29 +3094,35 @@
       <c r="C59" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D59" s="14">
+      <c r="D59" s="13">
         <v>204.09</v>
       </c>
-      <c r="E59" s="14">
+      <c r="E59" s="13">
         <v>202.88300000000001</v>
       </c>
-      <c r="F59" s="14">
+      <c r="F59" s="13">
         <v>202.81200000000001</v>
       </c>
-      <c r="G59" s="14">
+      <c r="G59" s="13">
         <v>202.94399999999999</v>
       </c>
-      <c r="H59" s="14">
+      <c r="H59" s="13">
         <v>202.82599999999999</v>
       </c>
-      <c r="I59" s="14">
+      <c r="I59" s="13">
         <v>202.94399999999999</v>
       </c>
-      <c r="J59" s="14">
+      <c r="J59" s="13">
         <v>202.82599999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59" s="13">
+        <v>202.45099999999999</v>
+      </c>
+      <c r="L59" s="13">
+        <v>202.27199999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="12"/>
       <c r="B60" s="3" t="s">
         <v>30</v>
@@ -2684,29 +3130,35 @@
       <c r="C60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D60" s="14">
+      <c r="D60" s="13">
         <v>277.41000000000003</v>
       </c>
-      <c r="E60" s="14">
+      <c r="E60" s="13">
         <v>200.32499999999999</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="13">
         <v>200.84800000000001</v>
       </c>
-      <c r="G60" s="14">
+      <c r="G60" s="13">
         <v>200.411</v>
       </c>
-      <c r="H60" s="14">
+      <c r="H60" s="13">
         <v>200.28200000000001</v>
       </c>
-      <c r="I60" s="14">
+      <c r="I60" s="13">
         <v>200.411</v>
       </c>
-      <c r="J60" s="14">
+      <c r="J60" s="13">
         <v>200.28200000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60" s="13">
+        <v>200</v>
+      </c>
+      <c r="L60" s="13">
+        <v>204.65799999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="12"/>
       <c r="B61" s="3" t="s">
         <v>31</v>
@@ -2714,29 +3166,31 @@
       <c r="C61" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D61" s="14">
+      <c r="D61" s="13">
         <v>100.629</v>
       </c>
-      <c r="E61" s="14">
+      <c r="E61" s="13">
         <v>105.006</v>
       </c>
-      <c r="F61" s="14">
+      <c r="F61" s="13">
         <v>114.072</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="13">
         <v>119.887</v>
       </c>
-      <c r="H61" s="14">
+      <c r="H61" s="13">
         <v>125.78</v>
       </c>
-      <c r="I61" s="14">
+      <c r="I61" s="13">
         <v>119.887</v>
       </c>
-      <c r="J61" s="14">
+      <c r="J61" s="13">
         <v>125.78</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="12"/>
       <c r="B62" s="3" t="s">
         <v>32</v>
@@ -2744,29 +3198,31 @@
       <c r="C62" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D62" s="14">
+      <c r="D62" s="13">
         <v>1335.66</v>
       </c>
-      <c r="E62" s="14">
+      <c r="E62" s="13">
         <v>422.56200000000001</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="13">
         <v>415.55799999999999</v>
       </c>
-      <c r="G62" s="14">
+      <c r="G62" s="13">
         <v>401.24599999999998</v>
       </c>
-      <c r="H62" s="14">
+      <c r="H62" s="13">
         <v>401.803</v>
       </c>
-      <c r="I62" s="14">
+      <c r="I62" s="13">
         <v>401.24599999999998</v>
       </c>
-      <c r="J62" s="14">
+      <c r="J62" s="13">
         <v>401.803</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" s="12"/>
       <c r="B63" s="3" t="s">
         <v>33</v>
@@ -2774,29 +3230,31 @@
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="14">
+      <c r="D63" s="13">
         <v>1326.7</v>
       </c>
-      <c r="E63" s="14">
+      <c r="E63" s="13">
         <v>474.11099999999999</v>
       </c>
-      <c r="F63" s="14">
+      <c r="F63" s="13">
         <v>475.97500000000002</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="13">
         <v>482.16500000000002</v>
       </c>
-      <c r="H63" s="14">
+      <c r="H63" s="13">
         <v>477.28899999999999</v>
       </c>
-      <c r="I63" s="14">
+      <c r="I63" s="13">
         <v>482.16500000000002</v>
       </c>
-      <c r="J63" s="14">
+      <c r="J63" s="13">
         <v>477.28899999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="12"/>
       <c r="B64" s="3" t="s">
         <v>34</v>
@@ -2804,29 +3262,31 @@
       <c r="C64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="14">
+      <c r="D64" s="13">
         <v>328446</v>
       </c>
-      <c r="E64" s="14">
+      <c r="E64" s="13">
         <v>44533.8</v>
       </c>
-      <c r="F64" s="14">
+      <c r="F64" s="13">
         <v>50368.2</v>
       </c>
-      <c r="G64" s="14">
+      <c r="G64" s="13">
         <v>1058.77</v>
       </c>
-      <c r="H64" s="14">
+      <c r="H64" s="13">
         <v>1157.3800000000001</v>
       </c>
-      <c r="I64" s="14">
+      <c r="I64" s="13">
         <v>1058.77</v>
       </c>
-      <c r="J64" s="14">
+      <c r="J64" s="13">
         <v>1157.3800000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="12"/>
       <c r="B65" s="3" t="s">
         <v>35</v>
@@ -2834,43 +3294,47 @@
       <c r="C65" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="14">
+      <c r="D65" s="13">
         <v>158276</v>
       </c>
-      <c r="E65" s="14">
+      <c r="E65" s="13">
         <v>7293.89</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F65" s="13">
         <v>8127.22</v>
       </c>
-      <c r="G65" s="14">
+      <c r="G65" s="13">
         <v>4581.91</v>
       </c>
-      <c r="H65" s="14">
+      <c r="H65" s="13">
         <v>4988.22</v>
       </c>
-      <c r="I65" s="14">
+      <c r="I65" s="13">
         <v>4581.91</v>
       </c>
-      <c r="J65" s="14">
+      <c r="J65" s="13">
         <v>4988.22</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="18">
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+    </row>
+    <row r="67" spans="1:12" ht="18">
       <c r="A67" s="3"/>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="22"/>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="2" t="s">
@@ -2897,8 +3361,14 @@
       <c r="J68" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="K68" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="L68" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" s="11" t="s">
         <v>36</v>
       </c>
@@ -2908,25 +3378,31 @@
       <c r="C69" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="14">
+      <c r="D69" s="13">
         <v>3437090000</v>
       </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14">
+      <c r="E69" s="13">
+        <v>33397800</v>
+      </c>
+      <c r="F69" s="13">
+        <v>30452600</v>
+      </c>
+      <c r="G69" s="13">
         <v>19634500</v>
       </c>
-      <c r="H69" s="14">
+      <c r="H69" s="13">
         <v>9802320</v>
       </c>
-      <c r="I69" s="14">
+      <c r="I69" s="13">
         <v>581847</v>
       </c>
-      <c r="J69" s="14">
+      <c r="J69" s="13">
         <v>191667</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" s="12"/>
       <c r="B70" s="3" t="s">
         <v>1</v>
@@ -2934,25 +3410,31 @@
       <c r="C70" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D70" s="14">
+      <c r="D70" s="13">
         <v>22292400000</v>
       </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14">
+      <c r="E70" s="13">
+        <v>11192.8</v>
+      </c>
+      <c r="F70" s="13">
+        <v>11553.5</v>
+      </c>
+      <c r="G70" s="13">
         <v>12455.3</v>
       </c>
-      <c r="H70" s="14">
+      <c r="H70" s="13">
         <v>12303.9</v>
       </c>
-      <c r="I70" s="14">
+      <c r="I70" s="13">
         <v>11576.6</v>
       </c>
-      <c r="J70" s="14">
+      <c r="J70" s="13">
         <v>2.6493900000000001E-13</v>
       </c>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" s="12"/>
       <c r="B71" s="3" t="s">
         <v>2</v>
@@ -2960,25 +3442,31 @@
       <c r="C71" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D71" s="14">
+      <c r="D71" s="13">
         <v>471270</v>
       </c>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14">
+      <c r="E71" s="13">
+        <v>155952</v>
+      </c>
+      <c r="F71" s="13">
+        <v>146478</v>
+      </c>
+      <c r="G71" s="13">
         <v>1.22038</v>
       </c>
-      <c r="H71" s="14">
+      <c r="H71" s="13">
         <v>1.1445299999999999E-3</v>
       </c>
-      <c r="I71" s="14">
+      <c r="I71" s="13">
         <v>75.422399999999996</v>
       </c>
-      <c r="J71" s="14">
+      <c r="J71" s="13">
         <v>515.31399999999996</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" s="11" t="s">
         <v>37</v>
       </c>
@@ -2988,25 +3476,31 @@
       <c r="C72" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D72" s="14">
+      <c r="D72" s="13">
         <v>2989.19</v>
       </c>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14">
+      <c r="E72" s="13">
+        <v>300.38099999999997</v>
+      </c>
+      <c r="F72" s="13">
+        <v>203.59800000000001</v>
+      </c>
+      <c r="G72" s="13">
         <v>326.755</v>
       </c>
-      <c r="H72" s="14">
+      <c r="H72" s="13">
         <v>196.679</v>
       </c>
-      <c r="I72" s="14">
+      <c r="I72" s="13">
         <v>271.38600000000002</v>
       </c>
-      <c r="J72" s="14">
+      <c r="J72" s="13">
         <v>166.06899999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" s="12"/>
       <c r="B73" s="3" t="s">
         <v>4</v>
@@ -3014,25 +3508,31 @@
       <c r="C73" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D73" s="14">
+      <c r="D73" s="13">
         <v>21.3184</v>
       </c>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14">
+      <c r="E73" s="13">
+        <v>21.313500000000001</v>
+      </c>
+      <c r="F73" s="13">
+        <v>21.307500000000001</v>
+      </c>
+      <c r="G73" s="13">
         <v>21.0642</v>
       </c>
-      <c r="H73" s="14">
+      <c r="H73" s="13">
         <v>21.059200000000001</v>
       </c>
-      <c r="I73" s="14">
+      <c r="I73" s="13">
         <v>20.632300000000001</v>
       </c>
-      <c r="J73" s="14">
+      <c r="J73" s="13">
         <v>20.626000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="12"/>
       <c r="B74" s="3" t="s">
         <v>5</v>
@@ -3040,25 +3540,31 @@
       <c r="C74" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D74" s="14">
+      <c r="D74" s="13">
         <v>149.59800000000001</v>
       </c>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14">
+      <c r="E74" s="13">
+        <v>5.5670500000000001</v>
+      </c>
+      <c r="F74" s="13">
+        <v>3.62453</v>
+      </c>
+      <c r="G74" s="13">
         <v>14.706200000000001</v>
       </c>
-      <c r="H74" s="14">
+      <c r="H74" s="13">
         <v>9.1156400000000009</v>
       </c>
-      <c r="I74" s="14">
+      <c r="I74" s="13">
         <v>27.047699999999999</v>
       </c>
-      <c r="J74" s="14">
+      <c r="J74" s="13">
         <v>5.5730700000000004</v>
       </c>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" s="12"/>
       <c r="B75" s="3" t="s">
         <v>6</v>
@@ -3066,25 +3572,31 @@
       <c r="C75" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D75" s="14">
+      <c r="D75" s="13">
         <v>148.22499999999999</v>
       </c>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14">
+      <c r="E75" s="13">
+        <v>1.02333E-3</v>
+      </c>
+      <c r="F75" s="13">
+        <v>1.8015E-6</v>
+      </c>
+      <c r="G75" s="13">
         <v>8.5169600000000005E-3</v>
       </c>
-      <c r="H75" s="14">
+      <c r="H75" s="13">
         <v>1.59038E-8</v>
       </c>
-      <c r="I75" s="14">
+      <c r="I75" s="13">
         <v>4.3886300000000001E-3</v>
       </c>
-      <c r="J75" s="14">
+      <c r="J75" s="13">
         <v>1.5238400000000001E-17</v>
       </c>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="12"/>
       <c r="B76" s="3" t="s">
         <v>7</v>
@@ -3092,25 +3604,31 @@
       <c r="C76" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D76" s="14">
+      <c r="D76" s="13">
         <v>847.10599999999999</v>
       </c>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14">
+      <c r="E76" s="13">
+        <v>645.18600000000004</v>
+      </c>
+      <c r="F76" s="13">
+        <v>632.87800000000004</v>
+      </c>
+      <c r="G76" s="13">
         <v>417.80200000000002</v>
       </c>
-      <c r="H76" s="14">
+      <c r="H76" s="13">
         <v>398.92700000000002</v>
       </c>
-      <c r="I76" s="14">
+      <c r="I76" s="13">
         <v>18.483699999999999</v>
       </c>
-      <c r="J76" s="14">
+      <c r="J76" s="13">
         <v>7.8391400000000004</v>
       </c>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" s="12"/>
       <c r="B77" s="3" t="s">
         <v>8</v>
@@ -3118,25 +3636,31 @@
       <c r="C77" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D77" s="14">
+      <c r="D77" s="13">
         <v>1061.67</v>
       </c>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14">
+      <c r="E77" s="13">
+        <v>760.16200000000003</v>
+      </c>
+      <c r="F77" s="13">
+        <v>747.46699999999998</v>
+      </c>
+      <c r="G77" s="13">
         <v>634.41999999999996</v>
       </c>
-      <c r="H77" s="14">
+      <c r="H77" s="13">
         <v>614.16800000000001</v>
       </c>
-      <c r="I77" s="14">
+      <c r="I77" s="13">
         <v>118.553</v>
       </c>
-      <c r="J77" s="14">
+      <c r="J77" s="13">
         <v>84.7453</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="12"/>
       <c r="B78" s="3" t="s">
         <v>9</v>
@@ -3144,25 +3668,31 @@
       <c r="C78" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D78" s="14">
+      <c r="D78" s="13">
         <v>25971</v>
       </c>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14">
+      <c r="E78" s="13">
+        <v>24969.599999999999</v>
+      </c>
+      <c r="F78" s="13">
+        <v>24924.5</v>
+      </c>
+      <c r="G78" s="13">
         <v>15939.7</v>
       </c>
-      <c r="H78" s="14">
+      <c r="H78" s="13">
         <v>15976.7</v>
       </c>
-      <c r="I78" s="14">
+      <c r="I78" s="13">
         <v>757.23099999999999</v>
       </c>
-      <c r="J78" s="14">
+      <c r="J78" s="13">
         <v>564.56399999999996</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" s="12"/>
       <c r="B79" s="3" t="s">
         <v>10</v>
@@ -3170,25 +3700,31 @@
       <c r="C79" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D79" s="14">
+      <c r="D79" s="13">
         <v>30281.7</v>
       </c>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14">
+      <c r="E79" s="13">
+        <v>29079.4</v>
+      </c>
+      <c r="F79" s="13">
+        <v>29111.5</v>
+      </c>
+      <c r="G79" s="13">
         <v>24309.200000000001</v>
       </c>
-      <c r="H79" s="14">
+      <c r="H79" s="13">
         <v>24399.1</v>
       </c>
-      <c r="I79" s="14">
+      <c r="I79" s="13">
         <v>12337.6</v>
       </c>
-      <c r="J79" s="14">
+      <c r="J79" s="13">
         <v>12244.6</v>
       </c>
-    </row>
-    <row r="80" spans="1:10">
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" s="12"/>
       <c r="B80" s="3" t="s">
         <v>11</v>
@@ -3196,25 +3732,31 @@
       <c r="C80" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D80" s="14">
+      <c r="D80" s="13">
         <v>3.9605199999999998</v>
       </c>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14">
+      <c r="E80" s="13">
+        <v>3.8563299999999998</v>
+      </c>
+      <c r="F80" s="13">
+        <v>3.7984300000000002</v>
+      </c>
+      <c r="G80" s="13">
         <v>2.0486800000000001</v>
       </c>
-      <c r="H80" s="14">
+      <c r="H80" s="13">
         <v>2.0386799999999998</v>
       </c>
-      <c r="I80" s="14">
+      <c r="I80" s="13">
         <v>0.52314799999999995</v>
       </c>
-      <c r="J80" s="14">
+      <c r="J80" s="13">
         <v>0.50453499999999996</v>
       </c>
-    </row>
-    <row r="81" spans="1:10">
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="12"/>
       <c r="B81" s="3" t="s">
         <v>12</v>
@@ -3222,25 +3764,31 @@
       <c r="C81" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D81" s="14">
+      <c r="D81" s="13">
         <v>0.82067900000000005</v>
       </c>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14">
+      <c r="E81" s="13">
+        <v>0.41922700000000002</v>
+      </c>
+      <c r="F81" s="13">
+        <v>0.43076799999999998</v>
+      </c>
+      <c r="G81" s="13">
         <v>0.41184799999999999</v>
       </c>
-      <c r="H81" s="14">
+      <c r="H81" s="13">
         <v>0.41424</v>
       </c>
-      <c r="I81" s="14">
+      <c r="I81" s="13">
         <v>0.31309999999999999</v>
       </c>
-      <c r="J81" s="14">
+      <c r="J81" s="13">
         <v>0.30676700000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="12"/>
       <c r="B82" s="3" t="s">
         <v>19</v>
@@ -3248,25 +3796,31 @@
       <c r="C82" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D82" s="14">
+      <c r="D82" s="13">
         <v>42.122199999999999</v>
       </c>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14">
+      <c r="E82" s="13">
+        <v>0.33149600000000001</v>
+      </c>
+      <c r="F82" s="13">
+        <v>0.34501900000000002</v>
+      </c>
+      <c r="G82" s="13">
         <v>0.32674799999999998</v>
       </c>
-      <c r="H82" s="14">
+      <c r="H82" s="13">
         <v>0.34407500000000002</v>
       </c>
-      <c r="I82" s="14">
+      <c r="I82" s="13">
         <v>0.28255599999999997</v>
       </c>
-      <c r="J82" s="14">
+      <c r="J82" s="13">
         <v>0.33541799999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="12"/>
       <c r="B83" s="3" t="s">
         <v>20</v>
@@ -3274,25 +3828,31 @@
       <c r="C83" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D83" s="14">
+      <c r="D83" s="13">
         <v>197945</v>
       </c>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14">
+      <c r="E83" s="13">
+        <v>68.248400000000004</v>
+      </c>
+      <c r="F83" s="13">
+        <v>67.565600000000003</v>
+      </c>
+      <c r="G83" s="13">
         <v>63.846899999999998</v>
       </c>
-      <c r="H83" s="14">
+      <c r="H83" s="13">
         <v>62.147500000000001</v>
       </c>
-      <c r="I83" s="14">
+      <c r="I83" s="13">
         <v>18.589099999999998</v>
       </c>
-      <c r="J83" s="14">
+      <c r="J83" s="13">
         <v>18.567299999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="12"/>
       <c r="B84" s="3" t="s">
         <v>21</v>
@@ -3300,25 +3860,31 @@
       <c r="C84" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D84" s="14">
+      <c r="D84" s="13">
         <v>46.834699999999998</v>
       </c>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14">
+      <c r="E84" s="13">
+        <v>46.237499999999997</v>
+      </c>
+      <c r="F84" s="13">
+        <v>46.218499999999999</v>
+      </c>
+      <c r="G84" s="13">
         <v>45.618099999999998</v>
       </c>
-      <c r="H84" s="14">
+      <c r="H84" s="13">
         <v>45.6068</v>
       </c>
-      <c r="I84" s="14">
+      <c r="I84" s="13">
         <v>40.415599999999998</v>
       </c>
-      <c r="J84" s="14">
+      <c r="J84" s="13">
         <v>40.205500000000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" s="11" t="s">
         <v>38</v>
       </c>
@@ -3328,25 +3894,31 @@
       <c r="C85" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D85" s="14">
+      <c r="D85" s="13">
         <v>272670000</v>
       </c>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14">
+      <c r="E85" s="13">
+        <v>7259550</v>
+      </c>
+      <c r="F85" s="13">
+        <v>7637710</v>
+      </c>
+      <c r="G85" s="13">
         <v>1128430</v>
       </c>
-      <c r="H85" s="14">
+      <c r="H85" s="13">
         <v>571479</v>
       </c>
-      <c r="I85" s="14">
+      <c r="I85" s="13">
         <v>4561.58</v>
       </c>
-      <c r="J85" s="14">
+      <c r="J85" s="13">
         <v>4545.1099999999997</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" s="12"/>
       <c r="B86" s="3" t="s">
         <v>23</v>
@@ -3354,25 +3926,31 @@
       <c r="C86" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D86" s="14">
+      <c r="D86" s="13">
         <v>163485</v>
       </c>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14">
+      <c r="E86" s="13">
+        <v>319.06</v>
+      </c>
+      <c r="F86" s="13">
+        <v>315.41500000000002</v>
+      </c>
+      <c r="G86" s="13">
         <v>317.68200000000002</v>
       </c>
-      <c r="H86" s="14">
+      <c r="H86" s="13">
         <v>314.55900000000003</v>
       </c>
-      <c r="I86" s="14">
+      <c r="I86" s="13">
         <v>227.024</v>
       </c>
-      <c r="J86" s="14">
+      <c r="J86" s="13">
         <v>238.78100000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="12"/>
       <c r="B87" s="3" t="s">
         <v>24</v>
@@ -3380,25 +3958,31 @@
       <c r="C87" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D87" s="14">
+      <c r="D87" s="13">
         <v>146.99100000000001</v>
       </c>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14">
+      <c r="E87" s="13">
+        <v>97.083100000000002</v>
+      </c>
+      <c r="F87" s="13">
+        <v>94.830500000000001</v>
+      </c>
+      <c r="G87" s="13">
         <v>96.432299999999998</v>
       </c>
-      <c r="H87" s="14">
+      <c r="H87" s="13">
         <v>95.471400000000003</v>
       </c>
-      <c r="I87" s="14">
+      <c r="I87" s="13">
         <v>94.557000000000002</v>
       </c>
-      <c r="J87" s="14">
+      <c r="J87" s="13">
         <v>94.67</v>
       </c>
-    </row>
-    <row r="88" spans="1:10">
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="12"/>
       <c r="B88" s="3" t="s">
         <v>25</v>
@@ -3406,25 +3990,31 @@
       <c r="C88" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D88" s="14">
+      <c r="D88" s="13">
         <v>275040</v>
       </c>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14">
+      <c r="E88" s="13">
+        <v>55195</v>
+      </c>
+      <c r="F88" s="13">
+        <v>50854.1</v>
+      </c>
+      <c r="G88" s="13">
         <v>400.00799999999998</v>
       </c>
-      <c r="H88" s="14">
+      <c r="H88" s="13">
         <v>397.90199999999999</v>
       </c>
-      <c r="I88" s="14">
+      <c r="I88" s="13">
         <v>244.49299999999999</v>
       </c>
-      <c r="J88" s="14">
+      <c r="J88" s="13">
         <v>169.70699999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:10">
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="12"/>
       <c r="B89" s="3" t="s">
         <v>26</v>
@@ -3432,25 +4022,31 @@
       <c r="C89" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D89" s="14">
+      <c r="D89" s="13">
         <v>120429000</v>
       </c>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14">
+      <c r="E89" s="13">
+        <v>5136570</v>
+      </c>
+      <c r="F89" s="13">
+        <v>5443450</v>
+      </c>
+      <c r="G89" s="13">
         <v>26166.1</v>
       </c>
-      <c r="H89" s="14">
+      <c r="H89" s="13">
         <v>13328.2</v>
       </c>
-      <c r="I89" s="14">
+      <c r="I89" s="13">
         <v>1964.13</v>
       </c>
-      <c r="J89" s="14">
+      <c r="J89" s="13">
         <v>2566.79</v>
       </c>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="12"/>
       <c r="B90" s="3" t="s">
         <v>27</v>
@@ -3458,25 +4054,31 @@
       <c r="C90" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D90" s="14">
+      <c r="D90" s="13">
         <v>4245.38</v>
       </c>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14">
+      <c r="E90" s="13">
+        <v>3520.69</v>
+      </c>
+      <c r="F90" s="13">
+        <v>3513.39</v>
+      </c>
+      <c r="G90" s="13">
         <v>3205.57</v>
       </c>
-      <c r="H90" s="14">
+      <c r="H90" s="13">
         <v>3147.39</v>
       </c>
-      <c r="I90" s="14">
+      <c r="I90" s="13">
         <v>1072.56</v>
       </c>
-      <c r="J90" s="14">
+      <c r="J90" s="13">
         <v>1108.8900000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" s="11" t="s">
         <v>39</v>
       </c>
@@ -3486,25 +4088,31 @@
       <c r="C91" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D91" s="14">
+      <c r="D91" s="13">
         <v>454.31099999999998</v>
       </c>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14">
+      <c r="E91" s="13">
+        <v>348.23599999999999</v>
+      </c>
+      <c r="F91" s="13">
         <v>348.23500000000001</v>
       </c>
-      <c r="H91" s="14">
+      <c r="G91" s="13">
         <v>348.23500000000001</v>
       </c>
-      <c r="I91" s="14">
+      <c r="H91" s="13">
         <v>348.23500000000001</v>
       </c>
-      <c r="J91" s="14">
+      <c r="I91" s="13">
         <v>348.23500000000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="J91" s="13">
+        <v>348.23500000000001</v>
+      </c>
+      <c r="K91" s="13"/>
+      <c r="L91" s="13"/>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="12"/>
       <c r="B92" s="3" t="s">
         <v>29</v>
@@ -3512,25 +4120,31 @@
       <c r="C92" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D92" s="14">
+      <c r="D92" s="13">
         <v>569.83399999999995</v>
       </c>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14">
+      <c r="E92" s="13">
+        <v>379.77800000000002</v>
+      </c>
+      <c r="F92" s="13">
+        <v>380.88499999999999</v>
+      </c>
+      <c r="G92" s="13">
         <v>382.541</v>
       </c>
-      <c r="H92" s="14">
+      <c r="H92" s="13">
         <v>383.57</v>
       </c>
-      <c r="I92" s="14">
+      <c r="I92" s="13">
         <v>387.92399999999998</v>
       </c>
-      <c r="J92" s="14">
+      <c r="J92" s="13">
         <v>391.70400000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="K92" s="13"/>
+      <c r="L92" s="13"/>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="12"/>
       <c r="B93" s="3" t="s">
         <v>30</v>
@@ -3538,25 +4152,31 @@
       <c r="C93" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D93" s="14">
+      <c r="D93" s="13">
         <v>700.90599999999995</v>
       </c>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14">
+      <c r="E93" s="13">
+        <v>200.00200000000001</v>
+      </c>
+      <c r="F93" s="13">
+        <v>200.001</v>
+      </c>
+      <c r="G93" s="13">
         <v>200.029</v>
       </c>
-      <c r="H93" s="14">
+      <c r="H93" s="13">
         <v>200.00200000000001</v>
       </c>
-      <c r="I93" s="14">
+      <c r="I93" s="13">
         <v>387.92399999999998</v>
       </c>
-      <c r="J93" s="14">
+      <c r="J93" s="13">
         <v>201.49600000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:10">
+      <c r="K93" s="13"/>
+      <c r="L93" s="13"/>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="12"/>
       <c r="B94" s="3" t="s">
         <v>31</v>
@@ -3564,25 +4184,31 @@
       <c r="C94" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D94" s="14">
+      <c r="D94" s="13">
         <v>304.92899999999997</v>
       </c>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14">
+      <c r="E94" s="13">
+        <v>200.309</v>
+      </c>
+      <c r="F94" s="13">
+        <v>200.42500000000001</v>
+      </c>
+      <c r="G94" s="13">
         <v>200.11699999999999</v>
       </c>
-      <c r="H94" s="14">
+      <c r="H94" s="13">
         <v>200.101</v>
       </c>
-      <c r="I94" s="14">
+      <c r="I94" s="13">
         <v>200</v>
       </c>
-      <c r="J94" s="14">
+      <c r="J94" s="13">
         <v>200.00299999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:10">
+      <c r="K94" s="13"/>
+      <c r="L94" s="13"/>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="12"/>
       <c r="B95" s="3" t="s">
         <v>32</v>
@@ -3590,21 +4216,31 @@
       <c r="C95" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D95" s="14">
+      <c r="D95" s="13">
         <v>3735.44</v>
       </c>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14">
+      <c r="E95" s="13">
+        <v>345.15899999999999</v>
+      </c>
+      <c r="F95" s="13">
+        <v>325.28699999999998</v>
+      </c>
+      <c r="G95" s="13">
         <v>413.73200000000003</v>
       </c>
-      <c r="H95" s="14">
+      <c r="H95" s="13">
         <v>344.87099999999998</v>
       </c>
-      <c r="I95" s="14"/>
-      <c r="J95" s="14"/>
-    </row>
-    <row r="96" spans="1:10">
+      <c r="I95" s="13">
+        <v>621.45299999999997</v>
+      </c>
+      <c r="J95" s="13">
+        <v>335.48599999999999</v>
+      </c>
+      <c r="K95" s="13"/>
+      <c r="L95" s="13"/>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="12"/>
       <c r="B96" s="3" t="s">
         <v>33</v>
@@ -3612,21 +4248,31 @@
       <c r="C96" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D96" s="14">
+      <c r="D96" s="13">
         <v>3533.33</v>
       </c>
-      <c r="E96" s="14"/>
-      <c r="F96" s="14"/>
-      <c r="G96" s="14">
+      <c r="E96" s="13">
+        <v>2142.4299999999998</v>
+      </c>
+      <c r="F96" s="13">
+        <v>2124.19</v>
+      </c>
+      <c r="G96" s="13">
         <v>2108.0100000000002</v>
       </c>
-      <c r="H96" s="14">
+      <c r="H96" s="13">
         <v>2103.2199999999998</v>
       </c>
-      <c r="I96" s="14"/>
-      <c r="J96" s="14"/>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="I96" s="13">
+        <v>2175.87</v>
+      </c>
+      <c r="J96" s="13">
+        <v>2228.73</v>
+      </c>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" s="12"/>
       <c r="B97" s="3" t="s">
         <v>34</v>
@@ -3634,19 +4280,31 @@
       <c r="C97" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D97" s="14">
+      <c r="D97" s="13">
         <v>857154</v>
       </c>
-      <c r="E97" s="14"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
-      <c r="H97" s="14">
+      <c r="E97" s="13">
+        <v>16084.1</v>
+      </c>
+      <c r="F97" s="13">
+        <v>11787.2</v>
+      </c>
+      <c r="G97" s="13">
+        <v>2235.4699999999998</v>
+      </c>
+      <c r="H97" s="13">
         <v>2152.46</v>
       </c>
-      <c r="I97" s="14"/>
-      <c r="J97" s="14"/>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="I97" s="13">
+        <v>812.53300000000002</v>
+      </c>
+      <c r="J97" s="13">
+        <v>1059.05</v>
+      </c>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="12"/>
       <c r="B98" s="3" t="s">
         <v>35</v>
@@ -3654,568 +4312,650 @@
       <c r="C98" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D98" s="14">
+      <c r="D98" s="13">
         <v>2598680</v>
       </c>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
-      <c r="I98" s="14"/>
-      <c r="J98" s="14"/>
-    </row>
-    <row r="100" spans="1:10" ht="18">
-      <c r="A100" s="3"/>
-      <c r="B100" s="13" t="s">
+      <c r="E98" s="13">
+        <v>10833.7</v>
+      </c>
+      <c r="F98" s="13">
+        <v>7762.71</v>
+      </c>
+      <c r="G98" s="13">
+        <v>10129.799999999999</v>
+      </c>
+      <c r="H98" s="13">
+        <v>7576.53</v>
+      </c>
+      <c r="I98" s="31">
+        <v>5833.25</v>
+      </c>
+      <c r="J98" s="13">
+        <v>8677.99</v>
+      </c>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+    </row>
+    <row r="100" spans="1:12" ht="18">
+      <c r="A100" s="23"/>
+      <c r="B100" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="2" t="s">
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
+      <c r="I100" s="25"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="26"/>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" s="23"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G101" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H101" s="2" t="s">
+      <c r="H101" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="I101" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="J101" s="2" t="s">
+      <c r="J101" s="27" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="11" t="s">
+      <c r="K101" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="L101" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="14"/>
-      <c r="H102" s="14"/>
-      <c r="I102" s="14"/>
-      <c r="J102" s="14"/>
-    </row>
-    <row r="103" spans="1:10">
-      <c r="A103" s="12"/>
-      <c r="B103" s="3" t="s">
+      <c r="D102" s="29"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="29"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="29"/>
+      <c r="K102" s="29"/>
+      <c r="L102" s="29"/>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103" s="30"/>
+      <c r="B103" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="14"/>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" s="12"/>
-      <c r="B104" s="3" t="s">
+      <c r="D103" s="29"/>
+      <c r="E103" s="29"/>
+      <c r="F103" s="29"/>
+      <c r="G103" s="29"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="29"/>
+      <c r="J103" s="29"/>
+      <c r="K103" s="29"/>
+      <c r="L103" s="29"/>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104" s="30"/>
+      <c r="B104" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C104" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="14"/>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="11" t="s">
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="29"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="29"/>
+      <c r="J104" s="29"/>
+      <c r="K104" s="29"/>
+      <c r="L104" s="29"/>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C105" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="14"/>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="12"/>
-      <c r="B106" s="3" t="s">
+      <c r="D105" s="29"/>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="29"/>
+      <c r="J105" s="29"/>
+      <c r="K105" s="29"/>
+      <c r="L105" s="29"/>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" s="30"/>
+      <c r="B106" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
-      <c r="J106" s="14"/>
-    </row>
-    <row r="107" spans="1:10">
-      <c r="A107" s="12"/>
-      <c r="B107" s="3" t="s">
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
+      <c r="K106" s="29"/>
+      <c r="L106" s="29"/>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" s="30"/>
+      <c r="B107" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="14"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="14"/>
-      <c r="J107" s="14"/>
-    </row>
-    <row r="108" spans="1:10">
-      <c r="A108" s="12"/>
-      <c r="B108" s="3" t="s">
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+      <c r="K107" s="29"/>
+      <c r="L107" s="29"/>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108" s="30"/>
+      <c r="B108" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D108" s="14"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="14"/>
-      <c r="G108" s="14"/>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
-      <c r="J108" s="14"/>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="12"/>
-      <c r="B109" s="3" t="s">
+      <c r="D108" s="29"/>
+      <c r="E108" s="29"/>
+      <c r="F108" s="29"/>
+      <c r="G108" s="29"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
+      <c r="J108" s="29"/>
+      <c r="K108" s="29"/>
+      <c r="L108" s="29"/>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" s="30"/>
+      <c r="B109" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14"/>
-      <c r="J109" s="14"/>
-    </row>
-    <row r="110" spans="1:10">
-      <c r="A110" s="12"/>
-      <c r="B110" s="3" t="s">
+      <c r="D109" s="29"/>
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+      <c r="G109" s="29"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="29"/>
+      <c r="J109" s="29"/>
+      <c r="K109" s="29"/>
+      <c r="L109" s="29"/>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110" s="30"/>
+      <c r="B110" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
-      <c r="H110" s="14"/>
-      <c r="I110" s="14"/>
-      <c r="J110" s="14"/>
-    </row>
-    <row r="111" spans="1:10">
-      <c r="A111" s="12"/>
-      <c r="B111" s="3" t="s">
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+      <c r="G110" s="29"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="29"/>
+      <c r="J110" s="29"/>
+      <c r="K110" s="29"/>
+      <c r="L110" s="29"/>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111" s="30"/>
+      <c r="B111" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
-      <c r="J111" s="14"/>
-    </row>
-    <row r="112" spans="1:10">
-      <c r="A112" s="12"/>
-      <c r="B112" s="3" t="s">
+      <c r="D111" s="29"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="29"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="29"/>
+      <c r="I111" s="29"/>
+      <c r="J111" s="29"/>
+      <c r="K111" s="29"/>
+      <c r="L111" s="29"/>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="A112" s="30"/>
+      <c r="B112" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
-      <c r="I112" s="14"/>
-      <c r="J112" s="14"/>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" s="12"/>
-      <c r="B113" s="3" t="s">
+      <c r="D112" s="29"/>
+      <c r="E112" s="29"/>
+      <c r="F112" s="29"/>
+      <c r="G112" s="29"/>
+      <c r="H112" s="29"/>
+      <c r="I112" s="29"/>
+      <c r="J112" s="29"/>
+      <c r="K112" s="29"/>
+      <c r="L112" s="29"/>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113" s="30"/>
+      <c r="B113" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
-      <c r="I113" s="14"/>
-      <c r="J113" s="14"/>
-    </row>
-    <row r="114" spans="1:10">
-      <c r="A114" s="12"/>
-      <c r="B114" s="3" t="s">
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="J113" s="29"/>
+      <c r="K113" s="29"/>
+      <c r="L113" s="29"/>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114" s="30"/>
+      <c r="B114" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
-      <c r="H114" s="14"/>
-      <c r="I114" s="14"/>
-      <c r="J114" s="14"/>
-    </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="12"/>
-      <c r="B115" s="3" t="s">
+      <c r="D114" s="29"/>
+      <c r="E114" s="29"/>
+      <c r="F114" s="29"/>
+      <c r="G114" s="29"/>
+      <c r="H114" s="29"/>
+      <c r="I114" s="29"/>
+      <c r="J114" s="29"/>
+      <c r="K114" s="29"/>
+      <c r="L114" s="29"/>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115" s="30"/>
+      <c r="B115" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C115" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
-      <c r="J115" s="14"/>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="12"/>
-      <c r="B116" s="3" t="s">
+      <c r="D115" s="29"/>
+      <c r="E115" s="29"/>
+      <c r="F115" s="29"/>
+      <c r="G115" s="29"/>
+      <c r="H115" s="29"/>
+      <c r="I115" s="29"/>
+      <c r="J115" s="29"/>
+      <c r="K115" s="29"/>
+      <c r="L115" s="29"/>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116" s="30"/>
+      <c r="B116" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D116" s="14"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14"/>
-      <c r="G116" s="14"/>
-      <c r="H116" s="14"/>
-      <c r="I116" s="14"/>
-      <c r="J116" s="14"/>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" s="12"/>
-      <c r="B117" s="3" t="s">
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
+      <c r="J116" s="29"/>
+      <c r="K116" s="29"/>
+      <c r="L116" s="29"/>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117" s="30"/>
+      <c r="B117" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D117" s="14"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14"/>
-      <c r="I117" s="14"/>
-      <c r="J117" s="14"/>
-    </row>
-    <row r="118" spans="1:10">
-      <c r="A118" s="11" t="s">
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="29"/>
+      <c r="K117" s="29"/>
+      <c r="L117" s="29"/>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C118" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D118" s="14"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
-      <c r="G118" s="14"/>
-      <c r="H118" s="14"/>
-      <c r="I118" s="14"/>
-      <c r="J118" s="14"/>
-    </row>
-    <row r="119" spans="1:10">
-      <c r="A119" s="12"/>
-      <c r="B119" s="3" t="s">
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
+      <c r="G118" s="29"/>
+      <c r="H118" s="29"/>
+      <c r="I118" s="29"/>
+      <c r="J118" s="29"/>
+      <c r="K118" s="29"/>
+      <c r="L118" s="29"/>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="30"/>
+      <c r="B119" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
-      <c r="H119" s="14"/>
-      <c r="I119" s="14"/>
-      <c r="J119" s="14"/>
-    </row>
-    <row r="120" spans="1:10">
-      <c r="A120" s="12"/>
-      <c r="B120" s="3" t="s">
+      <c r="D119" s="29"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="29"/>
+      <c r="G119" s="29"/>
+      <c r="H119" s="29"/>
+      <c r="I119" s="29"/>
+      <c r="J119" s="29"/>
+      <c r="K119" s="29"/>
+      <c r="L119" s="29"/>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="30"/>
+      <c r="B120" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
-      <c r="J120" s="14"/>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="A121" s="12"/>
-      <c r="B121" s="3" t="s">
+      <c r="D120" s="29"/>
+      <c r="E120" s="29"/>
+      <c r="F120" s="29"/>
+      <c r="G120" s="29"/>
+      <c r="H120" s="29"/>
+      <c r="I120" s="29"/>
+      <c r="J120" s="29"/>
+      <c r="K120" s="29"/>
+      <c r="L120" s="29"/>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" s="30"/>
+      <c r="B121" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="14"/>
-    </row>
-    <row r="122" spans="1:10">
-      <c r="A122" s="12"/>
-      <c r="B122" s="3" t="s">
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
+      <c r="G121" s="29"/>
+      <c r="H121" s="29"/>
+      <c r="I121" s="29"/>
+      <c r="J121" s="29"/>
+      <c r="K121" s="29"/>
+      <c r="L121" s="29"/>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="30"/>
+      <c r="B122" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D122" s="14"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
-      <c r="H122" s="14"/>
-      <c r="I122" s="14"/>
-      <c r="J122" s="14"/>
-    </row>
-    <row r="123" spans="1:10">
-      <c r="A123" s="12"/>
-      <c r="B123" s="3" t="s">
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="29"/>
+      <c r="G122" s="29"/>
+      <c r="H122" s="29"/>
+      <c r="I122" s="29"/>
+      <c r="J122" s="29"/>
+      <c r="K122" s="29"/>
+      <c r="L122" s="29"/>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" s="30"/>
+      <c r="B123" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
-      <c r="I123" s="14"/>
-      <c r="J123" s="14"/>
-    </row>
-    <row r="124" spans="1:10">
-      <c r="A124" s="11" t="s">
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="29"/>
+      <c r="K123" s="29"/>
+      <c r="L123" s="29"/>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C124" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D124" s="14"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
-      <c r="I124" s="14"/>
-      <c r="J124" s="14"/>
-    </row>
-    <row r="125" spans="1:10">
-      <c r="A125" s="12"/>
-      <c r="B125" s="3" t="s">
+      <c r="D124" s="29"/>
+      <c r="E124" s="29"/>
+      <c r="F124" s="29"/>
+      <c r="G124" s="29"/>
+      <c r="H124" s="29"/>
+      <c r="I124" s="29"/>
+      <c r="J124" s="29"/>
+      <c r="K124" s="29"/>
+      <c r="L124" s="29"/>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" s="30"/>
+      <c r="B125" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C125" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D125" s="14"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
-      <c r="I125" s="14"/>
-      <c r="J125" s="14"/>
-    </row>
-    <row r="126" spans="1:10">
-      <c r="A126" s="12"/>
-      <c r="B126" s="3" t="s">
+      <c r="D125" s="29"/>
+      <c r="E125" s="29"/>
+      <c r="F125" s="29"/>
+      <c r="G125" s="29"/>
+      <c r="H125" s="29"/>
+      <c r="I125" s="29"/>
+      <c r="J125" s="29"/>
+      <c r="K125" s="29"/>
+      <c r="L125" s="29"/>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" s="30"/>
+      <c r="B126" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="C126" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
-      <c r="I126" s="14"/>
-      <c r="J126" s="14"/>
-    </row>
-    <row r="127" spans="1:10">
-      <c r="A127" s="12"/>
-      <c r="B127" s="3" t="s">
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="29"/>
+      <c r="G126" s="29"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="29"/>
+      <c r="J126" s="29"/>
+      <c r="K126" s="29"/>
+      <c r="L126" s="29"/>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127" s="30"/>
+      <c r="B127" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D127" s="14"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
-      <c r="H127" s="14"/>
-      <c r="I127" s="14"/>
-      <c r="J127" s="14"/>
-    </row>
-    <row r="128" spans="1:10">
-      <c r="A128" s="12"/>
-      <c r="B128" s="3" t="s">
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
+      <c r="G127" s="29"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
+      <c r="J127" s="29"/>
+      <c r="K127" s="29"/>
+      <c r="L127" s="29"/>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" s="30"/>
+      <c r="B128" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C128" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D128" s="14"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
-      <c r="H128" s="14"/>
-      <c r="I128" s="14"/>
-      <c r="J128" s="14"/>
-    </row>
-    <row r="129" spans="1:10">
-      <c r="A129" s="12"/>
-      <c r="B129" s="3" t="s">
+      <c r="D128" s="29"/>
+      <c r="E128" s="29"/>
+      <c r="F128" s="29"/>
+      <c r="G128" s="29"/>
+      <c r="H128" s="29"/>
+      <c r="I128" s="29"/>
+      <c r="J128" s="29"/>
+      <c r="K128" s="29"/>
+      <c r="L128" s="29"/>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" s="30"/>
+      <c r="B129" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="C129" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
-      <c r="H129" s="14"/>
-      <c r="I129" s="14"/>
-      <c r="J129" s="14"/>
-    </row>
-    <row r="130" spans="1:10">
-      <c r="A130" s="12"/>
-      <c r="B130" s="3" t="s">
+      <c r="D129" s="29"/>
+      <c r="E129" s="29"/>
+      <c r="F129" s="29"/>
+      <c r="G129" s="29"/>
+      <c r="H129" s="29"/>
+      <c r="I129" s="29"/>
+      <c r="J129" s="29"/>
+      <c r="K129" s="29"/>
+      <c r="L129" s="29"/>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" s="30"/>
+      <c r="B130" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C130" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
-      <c r="H130" s="14"/>
-      <c r="I130" s="14"/>
-      <c r="J130" s="14"/>
-    </row>
-    <row r="131" spans="1:10">
-      <c r="A131" s="12"/>
-      <c r="B131" s="3" t="s">
+      <c r="D130" s="29"/>
+      <c r="E130" s="29"/>
+      <c r="F130" s="29"/>
+      <c r="G130" s="29"/>
+      <c r="H130" s="29"/>
+      <c r="I130" s="29"/>
+      <c r="J130" s="29"/>
+      <c r="K130" s="29"/>
+      <c r="L130" s="29"/>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" s="30"/>
+      <c r="B131" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C131" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D131" s="14"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
-      <c r="H131" s="14"/>
-      <c r="I131" s="14"/>
-      <c r="J131" s="14"/>
+      <c r="D131" s="29"/>
+      <c r="E131" s="29"/>
+      <c r="F131" s="29"/>
+      <c r="G131" s="29"/>
+      <c r="H131" s="29"/>
+      <c r="I131" s="29"/>
+      <c r="J131" s="29"/>
+      <c r="K131" s="29"/>
+      <c r="L131" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B100:J100"/>
     <mergeCell ref="A102:A104"/>
     <mergeCell ref="A105:A117"/>
     <mergeCell ref="A118:A123"/>
     <mergeCell ref="A124:A131"/>
-    <mergeCell ref="B67:J67"/>
+    <mergeCell ref="B100:L100"/>
     <mergeCell ref="A69:A71"/>
     <mergeCell ref="A72:A84"/>
     <mergeCell ref="A85:A90"/>
     <mergeCell ref="A91:A98"/>
-    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B67:L67"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A51"/>
     <mergeCell ref="A52:A57"/>
     <mergeCell ref="A58:A65"/>
+    <mergeCell ref="B34:L34"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A18"/>
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>